<commit_message>
Completeion of id tag persName
</commit_message>
<xml_diff>
--- a/Kate.CheckList.MT.xlsx
+++ b/Kate.CheckList.MT.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="530">
   <si>
     <t>MpÃ©pe (1)</t>
   </si>
@@ -1608,6 +1608,12 @@
   </si>
   <si>
     <t>Query</t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>query</t>
   </si>
 </sst>
 </file>
@@ -1927,8 +1933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D518"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="C213" sqref="C213"/>
+    <sheetView tabSelected="1" topLeftCell="B106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1949,7 +1955,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -1957,7 +1963,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
@@ -2367,6 +2373,9 @@
       <c r="B55" t="s">
         <v>53</v>
       </c>
+      <c r="C55" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
@@ -2388,6 +2397,9 @@
       <c r="B58" t="s">
         <v>56</v>
       </c>
+      <c r="C58" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
@@ -2693,7 +2705,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>95</v>
       </c>
@@ -2701,7 +2713,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>96</v>
       </c>
@@ -2709,7 +2721,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>97</v>
       </c>
@@ -2717,17 +2729,23 @@
         <v>517</v>
       </c>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C100" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D101" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>100</v>
       </c>
@@ -2735,7 +2753,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>101</v>
       </c>
@@ -2743,7 +2761,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>102</v>
       </c>
@@ -2751,7 +2769,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>103</v>
       </c>
@@ -2759,7 +2777,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>104</v>
       </c>
@@ -2767,7 +2785,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>105</v>
       </c>
@@ -2775,12 +2793,15 @@
         <v>517</v>
       </c>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C108" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>107</v>
       </c>
@@ -2788,7 +2809,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>108</v>
       </c>
@@ -2796,7 +2817,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>109</v>
       </c>
@@ -2804,7 +2825,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>110</v>
       </c>
@@ -2812,7 +2833,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>111</v>
       </c>
@@ -2820,7 +2841,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>112</v>
       </c>
@@ -2828,7 +2849,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>113</v>
       </c>
@@ -2836,7 +2857,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>114</v>
       </c>
@@ -2844,12 +2865,15 @@
         <v>517</v>
       </c>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D117" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>116</v>
       </c>
@@ -2857,7 +2881,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>117</v>
       </c>
@@ -2865,7 +2889,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>118</v>
       </c>
@@ -2873,7 +2897,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>119</v>
       </c>
@@ -2881,7 +2905,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>120</v>
       </c>
@@ -2889,7 +2913,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>121</v>
       </c>
@@ -2897,12 +2921,15 @@
         <v>517</v>
       </c>
     </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D124" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>123</v>
       </c>
@@ -2910,7 +2937,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>124</v>
       </c>
@@ -2918,7 +2945,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>125</v>
       </c>
@@ -2926,7 +2953,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>126</v>
       </c>
@@ -2994,11 +3021,17 @@
       <c r="B136" t="s">
         <v>134</v>
       </c>
+      <c r="C136" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>135</v>
       </c>
+      <c r="C137" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
@@ -3092,56 +3125,89 @@
       <c r="B149" t="s">
         <v>147</v>
       </c>
+      <c r="C149" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="150" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
         <v>148</v>
       </c>
+      <c r="C150" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="151" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
         <v>149</v>
       </c>
+      <c r="C151" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
         <v>150</v>
       </c>
+      <c r="C152" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="153" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
         <v>151</v>
       </c>
+      <c r="C153" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="154" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
         <v>152</v>
       </c>
+      <c r="C154" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="155" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
         <v>153</v>
       </c>
+      <c r="C155" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="156" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
         <v>154</v>
       </c>
+      <c r="C156" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="157" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
         <v>155</v>
       </c>
+      <c r="C157" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="158" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
         <v>156</v>
       </c>
+      <c r="C158" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="159" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
         <v>157</v>
       </c>
+      <c r="C159" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="160" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
@@ -3151,62 +3217,95 @@
         <v>517</v>
       </c>
     </row>
-    <row r="161" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C161" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C162" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C163" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="164" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="165" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C164" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="166" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C165" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C166" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="167" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D167" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="168" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="169" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C168" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="169" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="170" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C169" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="170" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="171" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C170" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C171" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="172" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
         <v>170</v>
       </c>
@@ -3214,72 +3313,111 @@
         <v>517</v>
       </c>
     </row>
-    <row r="173" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="174" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C173" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="174" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="175" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C174" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="175" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="176" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C175" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C176" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C177" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="179" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C178" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="180" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C179" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="180" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="181" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C180" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="182" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C181" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="183" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C182" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="183" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="184" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C183" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="185" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C184" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="185" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="186" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C185" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="186" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
         <v>184</v>
       </c>
@@ -3287,85 +3425,133 @@
         <v>517</v>
       </c>
     </row>
-    <row r="187" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="188" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C187" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="188" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="189" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C188" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="189" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="190" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C189" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="190" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="191" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C190" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="191" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="192" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D191" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="192" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
         <v>190</v>
+      </c>
+      <c r="C192" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="193" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
         <v>191</v>
       </c>
+      <c r="C193" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="194" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
         <v>192</v>
       </c>
+      <c r="C194" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="195" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
         <v>193</v>
       </c>
+      <c r="C195" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="196" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
         <v>194</v>
       </c>
+      <c r="C196" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="197" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
         <v>195</v>
       </c>
+      <c r="C197" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="198" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
         <v>196</v>
       </c>
+      <c r="C198" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="199" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
         <v>197</v>
       </c>
+      <c r="C199" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="200" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
         <v>198</v>
       </c>
+      <c r="C200" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="201" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
         <v>199</v>
       </c>
+      <c r="C201" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="202" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
         <v>200</v>
       </c>
+      <c r="C202" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="203" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
@@ -3379,46 +3565,73 @@
       <c r="B204" t="s">
         <v>202</v>
       </c>
+      <c r="C204" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="205" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B205" t="s">
         <v>203</v>
       </c>
+      <c r="C205" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="206" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
         <v>204</v>
       </c>
+      <c r="C206" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="207" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
         <v>205</v>
       </c>
+      <c r="C207" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="208" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
         <v>206</v>
       </c>
+      <c r="C208" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="209" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
         <v>207</v>
       </c>
+      <c r="C209" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="210" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B210" t="s">
         <v>208</v>
       </c>
+      <c r="C210" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="211" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B211" t="s">
         <v>209</v>
       </c>
+      <c r="C211" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="212" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
         <v>210</v>
       </c>
+      <c r="C212" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="213" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B213" t="s">
@@ -3688,6 +3901,9 @@
       <c r="B246" t="s">
         <v>244</v>
       </c>
+      <c r="C246" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="247" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B247" t="s">
@@ -4117,6 +4333,9 @@
       <c r="B300" t="s">
         <v>298</v>
       </c>
+      <c r="D300" t="s">
+        <v>526</v>
+      </c>
     </row>
     <row r="301" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B301" t="s">
@@ -4154,6 +4373,9 @@
       <c r="B305" t="s">
         <v>0</v>
       </c>
+      <c r="C305" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="306" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B306" t="s">
@@ -4863,6 +5085,9 @@
       <c r="B394" t="s">
         <v>391</v>
       </c>
+      <c r="C394" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="395" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B395" t="s">
@@ -5119,6 +5344,9 @@
       <c r="B426" t="s">
         <v>423</v>
       </c>
+      <c r="C426" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="427" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B427" t="s">
@@ -5156,6 +5384,9 @@
       <c r="B431" t="s">
         <v>428</v>
       </c>
+      <c r="C431" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="432" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B432" t="s">
@@ -5201,6 +5432,9 @@
       <c r="B437" t="s">
         <v>434</v>
       </c>
+      <c r="C437" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="438" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B438" t="s">
@@ -5262,6 +5496,9 @@
       <c r="B445" t="s">
         <v>442</v>
       </c>
+      <c r="C445" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="446" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B446" t="s">
@@ -5287,7 +5524,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="449" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="449" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B449" t="s">
         <v>446</v>
       </c>
@@ -5295,7 +5532,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="450" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="450" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B450" t="s">
         <v>447</v>
       </c>
@@ -5303,12 +5540,15 @@
         <v>517</v>
       </c>
     </row>
-    <row r="451" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="451" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B451" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="452" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C451" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="452" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B452" t="s">
         <v>449</v>
       </c>
@@ -5316,7 +5556,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="453" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="453" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B453" t="s">
         <v>450</v>
       </c>
@@ -5324,7 +5564,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="454" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="454" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B454" t="s">
         <v>451</v>
       </c>
@@ -5332,7 +5572,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="455" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="455" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B455" t="s">
         <v>452</v>
       </c>
@@ -5340,7 +5580,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="456" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="456" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B456" t="s">
         <v>453</v>
       </c>
@@ -5348,7 +5588,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="457" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="457" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B457" t="s">
         <v>454</v>
       </c>
@@ -5356,15 +5596,15 @@
         <v>517</v>
       </c>
     </row>
-    <row r="458" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="458" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B458" t="s">
         <v>455</v>
       </c>
       <c r="C458" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="459" spans="2:3" x14ac:dyDescent="0.25">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="459" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B459" t="s">
         <v>456</v>
       </c>
@@ -5372,7 +5612,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="460" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="460" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B460" t="s">
         <v>457</v>
       </c>
@@ -5380,15 +5620,18 @@
         <v>517</v>
       </c>
     </row>
-    <row r="461" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="461" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B461" t="s">
         <v>458</v>
       </c>
       <c r="C461" t="s">
+        <v>528</v>
+      </c>
+      <c r="D461" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="462" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="462" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B462" t="s">
         <v>459</v>
       </c>
@@ -5396,7 +5639,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="463" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="463" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B463" t="s">
         <v>460</v>
       </c>
@@ -5404,7 +5647,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="464" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="464" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B464" t="s">
         <v>461</v>
       </c>
@@ -5727,6 +5970,9 @@
     <row r="504" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B504" t="s">
         <v>501</v>
+      </c>
+      <c r="C504" t="s">
+        <v>528</v>
       </c>
       <c r="D504" t="s">
         <v>522</v>

</xml_diff>

<commit_message>
Revert "Completeion of id tag persName"
This reverts commit 396e2871161094b33653aa93314237261e70254b.
</commit_message>
<xml_diff>
--- a/Kate.CheckList.MT.xlsx
+++ b/Kate.CheckList.MT.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="528">
   <si>
     <t>MpÃ©pe (1)</t>
   </si>
@@ -1608,12 +1608,6 @@
   </si>
   <si>
     <t>Query</t>
-  </si>
-  <si>
-    <t>ND</t>
-  </si>
-  <si>
-    <t>query</t>
   </si>
 </sst>
 </file>
@@ -1933,8 +1927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D518"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="C213" sqref="C213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1955,7 +1949,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -1963,7 +1957,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
@@ -2373,9 +2367,6 @@
       <c r="B55" t="s">
         <v>53</v>
       </c>
-      <c r="C55" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
@@ -2397,9 +2388,6 @@
       <c r="B58" t="s">
         <v>56</v>
       </c>
-      <c r="C58" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
@@ -2705,7 +2693,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>95</v>
       </c>
@@ -2713,7 +2701,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>96</v>
       </c>
@@ -2721,7 +2709,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>97</v>
       </c>
@@ -2729,23 +2717,17 @@
         <v>517</v>
       </c>
     </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>98</v>
       </c>
-      <c r="C100" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>99</v>
       </c>
-      <c r="D101" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>100</v>
       </c>
@@ -2753,7 +2735,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>101</v>
       </c>
@@ -2761,7 +2743,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>102</v>
       </c>
@@ -2769,7 +2751,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>103</v>
       </c>
@@ -2777,7 +2759,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>104</v>
       </c>
@@ -2785,7 +2767,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>105</v>
       </c>
@@ -2793,15 +2775,12 @@
         <v>517</v>
       </c>
     </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>106</v>
       </c>
-      <c r="C108" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>107</v>
       </c>
@@ -2809,7 +2788,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>108</v>
       </c>
@@ -2817,7 +2796,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>109</v>
       </c>
@@ -2825,7 +2804,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>110</v>
       </c>
@@ -2833,7 +2812,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>111</v>
       </c>
@@ -2841,7 +2820,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>112</v>
       </c>
@@ -2849,7 +2828,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>113</v>
       </c>
@@ -2857,7 +2836,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>114</v>
       </c>
@@ -2865,15 +2844,12 @@
         <v>517</v>
       </c>
     </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>115</v>
       </c>
-      <c r="D117" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>116</v>
       </c>
@@ -2881,7 +2857,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>117</v>
       </c>
@@ -2889,7 +2865,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>118</v>
       </c>
@@ -2897,7 +2873,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>119</v>
       </c>
@@ -2905,7 +2881,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>120</v>
       </c>
@@ -2913,7 +2889,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>121</v>
       </c>
@@ -2921,15 +2897,12 @@
         <v>517</v>
       </c>
     </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>122</v>
       </c>
-      <c r="D124" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>123</v>
       </c>
@@ -2937,7 +2910,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>124</v>
       </c>
@@ -2945,7 +2918,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>125</v>
       </c>
@@ -2953,7 +2926,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>126</v>
       </c>
@@ -3021,17 +2994,11 @@
       <c r="B136" t="s">
         <v>134</v>
       </c>
-      <c r="C136" t="s">
-        <v>528</v>
-      </c>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>135</v>
       </c>
-      <c r="C137" t="s">
-        <v>528</v>
-      </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
@@ -3125,89 +3092,56 @@
       <c r="B149" t="s">
         <v>147</v>
       </c>
-      <c r="C149" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="150" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
         <v>148</v>
       </c>
-      <c r="C150" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="151" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
         <v>149</v>
       </c>
-      <c r="C151" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
         <v>150</v>
       </c>
-      <c r="C152" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="153" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
         <v>151</v>
       </c>
-      <c r="C153" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="154" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
         <v>152</v>
       </c>
-      <c r="C154" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="155" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
         <v>153</v>
       </c>
-      <c r="C155" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="156" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
         <v>154</v>
       </c>
-      <c r="C156" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="157" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
         <v>155</v>
       </c>
-      <c r="C157" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="158" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
         <v>156</v>
       </c>
-      <c r="C158" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="159" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
         <v>157</v>
       </c>
-      <c r="C159" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="160" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
@@ -3217,95 +3151,62 @@
         <v>517</v>
       </c>
     </row>
-    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
         <v>159</v>
       </c>
-      <c r="C161" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
         <v>160</v>
       </c>
-      <c r="C162" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
         <v>161</v>
       </c>
-      <c r="C163" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="164" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
         <v>162</v>
       </c>
-      <c r="C164" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="165" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
         <v>163</v>
       </c>
-      <c r="C165" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="166" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
         <v>164</v>
       </c>
-      <c r="C166" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="167" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
         <v>165</v>
       </c>
-      <c r="D167" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="168" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
         <v>166</v>
       </c>
-      <c r="C168" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="169" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="169" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
         <v>167</v>
       </c>
-      <c r="C169" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="170" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="170" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
         <v>168</v>
       </c>
-      <c r="C170" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="171" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
         <v>169</v>
       </c>
-      <c r="C171" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="172" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
         <v>170</v>
       </c>
@@ -3313,111 +3214,72 @@
         <v>517</v>
       </c>
     </row>
-    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
         <v>171</v>
       </c>
-      <c r="C173" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="174" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="174" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
         <v>172</v>
       </c>
-      <c r="C174" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="175" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="175" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
         <v>173</v>
       </c>
-      <c r="C175" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="176" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
         <v>174</v>
       </c>
-      <c r="C176" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
         <v>175</v>
       </c>
-      <c r="C177" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
         <v>176</v>
       </c>
-      <c r="C178" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="179" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
         <v>177</v>
       </c>
-      <c r="C179" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="180" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="180" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
         <v>178</v>
       </c>
-      <c r="C180" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="181" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
         <v>179</v>
       </c>
-      <c r="C181" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="182" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
         <v>180</v>
       </c>
-      <c r="C182" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="183" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="183" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
         <v>181</v>
       </c>
-      <c r="C183" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="184" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
         <v>182</v>
       </c>
-      <c r="C184" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="185" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="185" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
         <v>183</v>
       </c>
-      <c r="C185" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="186" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="186" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
         <v>184</v>
       </c>
@@ -3425,133 +3287,85 @@
         <v>517</v>
       </c>
     </row>
-    <row r="187" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
         <v>185</v>
       </c>
-      <c r="C187" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="188" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="188" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
         <v>186</v>
       </c>
-      <c r="C188" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="189" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="189" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
         <v>187</v>
       </c>
-      <c r="C189" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="190" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="190" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
         <v>188</v>
       </c>
-      <c r="C190" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="191" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="191" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
         <v>189</v>
       </c>
-      <c r="D191" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="192" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="192" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
         <v>190</v>
-      </c>
-      <c r="C192" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="193" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
         <v>191</v>
       </c>
-      <c r="C193" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="194" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
         <v>192</v>
       </c>
-      <c r="C194" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="195" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
         <v>193</v>
       </c>
-      <c r="C195" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="196" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
         <v>194</v>
       </c>
-      <c r="C196" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="197" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
         <v>195</v>
       </c>
-      <c r="C197" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="198" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
         <v>196</v>
       </c>
-      <c r="C198" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="199" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
         <v>197</v>
       </c>
-      <c r="C199" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="200" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
         <v>198</v>
       </c>
-      <c r="C200" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="201" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
         <v>199</v>
       </c>
-      <c r="C201" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="202" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
         <v>200</v>
       </c>
-      <c r="C202" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="203" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
@@ -3565,73 +3379,46 @@
       <c r="B204" t="s">
         <v>202</v>
       </c>
-      <c r="C204" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="205" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B205" t="s">
         <v>203</v>
       </c>
-      <c r="C205" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="206" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
         <v>204</v>
       </c>
-      <c r="C206" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="207" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
         <v>205</v>
       </c>
-      <c r="C207" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="208" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
         <v>206</v>
       </c>
-      <c r="C208" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="209" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
         <v>207</v>
       </c>
-      <c r="C209" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="210" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B210" t="s">
         <v>208</v>
       </c>
-      <c r="C210" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="211" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B211" t="s">
         <v>209</v>
       </c>
-      <c r="C211" t="s">
-        <v>528</v>
-      </c>
     </row>
     <row r="212" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
         <v>210</v>
       </c>
-      <c r="C212" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="213" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B213" t="s">
@@ -3901,9 +3688,6 @@
       <c r="B246" t="s">
         <v>244</v>
       </c>
-      <c r="C246" t="s">
-        <v>528</v>
-      </c>
     </row>
     <row r="247" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B247" t="s">
@@ -4333,9 +4117,6 @@
       <c r="B300" t="s">
         <v>298</v>
       </c>
-      <c r="D300" t="s">
-        <v>526</v>
-      </c>
     </row>
     <row r="301" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B301" t="s">
@@ -4373,9 +4154,6 @@
       <c r="B305" t="s">
         <v>0</v>
       </c>
-      <c r="C305" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="306" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B306" t="s">
@@ -5085,9 +4863,6 @@
       <c r="B394" t="s">
         <v>391</v>
       </c>
-      <c r="C394" t="s">
-        <v>528</v>
-      </c>
     </row>
     <row r="395" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B395" t="s">
@@ -5344,9 +5119,6 @@
       <c r="B426" t="s">
         <v>423</v>
       </c>
-      <c r="C426" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="427" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B427" t="s">
@@ -5384,9 +5156,6 @@
       <c r="B431" t="s">
         <v>428</v>
       </c>
-      <c r="C431" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="432" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B432" t="s">
@@ -5432,9 +5201,6 @@
       <c r="B437" t="s">
         <v>434</v>
       </c>
-      <c r="C437" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="438" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B438" t="s">
@@ -5496,9 +5262,6 @@
       <c r="B445" t="s">
         <v>442</v>
       </c>
-      <c r="C445" t="s">
-        <v>517</v>
-      </c>
     </row>
     <row r="446" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B446" t="s">
@@ -5524,7 +5287,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="449" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="449" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B449" t="s">
         <v>446</v>
       </c>
@@ -5532,7 +5295,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="450" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="450" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B450" t="s">
         <v>447</v>
       </c>
@@ -5540,15 +5303,12 @@
         <v>517</v>
       </c>
     </row>
-    <row r="451" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="451" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B451" t="s">
         <v>448</v>
       </c>
-      <c r="C451" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="452" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="452" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B452" t="s">
         <v>449</v>
       </c>
@@ -5556,7 +5316,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="453" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="453" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B453" t="s">
         <v>450</v>
       </c>
@@ -5564,7 +5324,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="454" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="454" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B454" t="s">
         <v>451</v>
       </c>
@@ -5572,7 +5332,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="455" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="455" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B455" t="s">
         <v>452</v>
       </c>
@@ -5580,7 +5340,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="456" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="456" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B456" t="s">
         <v>453</v>
       </c>
@@ -5588,7 +5348,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="457" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="457" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B457" t="s">
         <v>454</v>
       </c>
@@ -5596,15 +5356,15 @@
         <v>517</v>
       </c>
     </row>
-    <row r="458" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="458" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B458" t="s">
         <v>455</v>
       </c>
       <c r="C458" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="459" spans="2:4" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="459" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B459" t="s">
         <v>456</v>
       </c>
@@ -5612,7 +5372,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="460" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="460" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B460" t="s">
         <v>457</v>
       </c>
@@ -5620,18 +5380,15 @@
         <v>517</v>
       </c>
     </row>
-    <row r="461" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="461" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B461" t="s">
         <v>458</v>
       </c>
       <c r="C461" t="s">
-        <v>528</v>
-      </c>
-      <c r="D461" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="462" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="462" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B462" t="s">
         <v>459</v>
       </c>
@@ -5639,7 +5396,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="463" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="463" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B463" t="s">
         <v>460</v>
       </c>
@@ -5647,7 +5404,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="464" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="464" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B464" t="s">
         <v>461</v>
       </c>
@@ -5970,9 +5727,6 @@
     <row r="504" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B504" t="s">
         <v>501</v>
-      </c>
-      <c r="C504" t="s">
-        <v>528</v>
       </c>
       <c r="D504" t="s">
         <v>522</v>

</xml_diff>

<commit_message>
Revert "Revert "Completeion of id tag persName""
This reverts commit a06caeaf0d81955d3b5273e495bf661b06faeca9.
</commit_message>
<xml_diff>
--- a/Kate.CheckList.MT.xlsx
+++ b/Kate.CheckList.MT.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="530">
   <si>
     <t>MpÃ©pe (1)</t>
   </si>
@@ -1608,6 +1608,12 @@
   </si>
   <si>
     <t>Query</t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>query</t>
   </si>
 </sst>
 </file>
@@ -1927,8 +1933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D518"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="C213" sqref="C213"/>
+    <sheetView tabSelected="1" topLeftCell="B106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1949,7 +1955,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -1957,7 +1963,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
@@ -2367,6 +2373,9 @@
       <c r="B55" t="s">
         <v>53</v>
       </c>
+      <c r="C55" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
@@ -2388,6 +2397,9 @@
       <c r="B58" t="s">
         <v>56</v>
       </c>
+      <c r="C58" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
@@ -2693,7 +2705,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>95</v>
       </c>
@@ -2701,7 +2713,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>96</v>
       </c>
@@ -2709,7 +2721,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>97</v>
       </c>
@@ -2717,17 +2729,23 @@
         <v>517</v>
       </c>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C100" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D101" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>100</v>
       </c>
@@ -2735,7 +2753,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>101</v>
       </c>
@@ -2743,7 +2761,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>102</v>
       </c>
@@ -2751,7 +2769,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>103</v>
       </c>
@@ -2759,7 +2777,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>104</v>
       </c>
@@ -2767,7 +2785,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>105</v>
       </c>
@@ -2775,12 +2793,15 @@
         <v>517</v>
       </c>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C108" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>107</v>
       </c>
@@ -2788,7 +2809,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>108</v>
       </c>
@@ -2796,7 +2817,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>109</v>
       </c>
@@ -2804,7 +2825,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>110</v>
       </c>
@@ -2812,7 +2833,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>111</v>
       </c>
@@ -2820,7 +2841,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>112</v>
       </c>
@@ -2828,7 +2849,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>113</v>
       </c>
@@ -2836,7 +2857,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>114</v>
       </c>
@@ -2844,12 +2865,15 @@
         <v>517</v>
       </c>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D117" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>116</v>
       </c>
@@ -2857,7 +2881,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>117</v>
       </c>
@@ -2865,7 +2889,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>118</v>
       </c>
@@ -2873,7 +2897,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>119</v>
       </c>
@@ -2881,7 +2905,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>120</v>
       </c>
@@ -2889,7 +2913,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>121</v>
       </c>
@@ -2897,12 +2921,15 @@
         <v>517</v>
       </c>
     </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D124" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>123</v>
       </c>
@@ -2910,7 +2937,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>124</v>
       </c>
@@ -2918,7 +2945,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>125</v>
       </c>
@@ -2926,7 +2953,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>126</v>
       </c>
@@ -2994,11 +3021,17 @@
       <c r="B136" t="s">
         <v>134</v>
       </c>
+      <c r="C136" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>135</v>
       </c>
+      <c r="C137" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
@@ -3092,56 +3125,89 @@
       <c r="B149" t="s">
         <v>147</v>
       </c>
+      <c r="C149" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="150" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
         <v>148</v>
       </c>
+      <c r="C150" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="151" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
         <v>149</v>
       </c>
+      <c r="C151" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
         <v>150</v>
       </c>
+      <c r="C152" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="153" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
         <v>151</v>
       </c>
+      <c r="C153" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="154" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
         <v>152</v>
       </c>
+      <c r="C154" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="155" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
         <v>153</v>
       </c>
+      <c r="C155" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="156" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
         <v>154</v>
       </c>
+      <c r="C156" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="157" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
         <v>155</v>
       </c>
+      <c r="C157" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="158" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
         <v>156</v>
       </c>
+      <c r="C158" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="159" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
         <v>157</v>
       </c>
+      <c r="C159" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="160" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
@@ -3151,62 +3217,95 @@
         <v>517</v>
       </c>
     </row>
-    <row r="161" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C161" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C162" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C163" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="164" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="165" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C164" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="166" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C165" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C166" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="167" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D167" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="168" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="169" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C168" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="169" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="170" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C169" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="170" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="171" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C170" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C171" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="172" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
         <v>170</v>
       </c>
@@ -3214,72 +3313,111 @@
         <v>517</v>
       </c>
     </row>
-    <row r="173" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="174" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C173" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="174" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="175" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C174" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="175" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="176" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C175" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C176" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C177" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="179" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C178" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="180" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C179" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="180" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="181" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C180" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="182" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C181" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="183" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C182" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="183" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="184" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C183" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="185" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C184" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="185" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="186" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C185" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="186" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
         <v>184</v>
       </c>
@@ -3287,85 +3425,133 @@
         <v>517</v>
       </c>
     </row>
-    <row r="187" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="188" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C187" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="188" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="189" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C188" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="189" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="190" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C189" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="190" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="191" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C190" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="191" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="192" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D191" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="192" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
         <v>190</v>
+      </c>
+      <c r="C192" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="193" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
         <v>191</v>
       </c>
+      <c r="C193" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="194" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
         <v>192</v>
       </c>
+      <c r="C194" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="195" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
         <v>193</v>
       </c>
+      <c r="C195" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="196" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
         <v>194</v>
       </c>
+      <c r="C196" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="197" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
         <v>195</v>
       </c>
+      <c r="C197" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="198" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
         <v>196</v>
       </c>
+      <c r="C198" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="199" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
         <v>197</v>
       </c>
+      <c r="C199" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="200" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
         <v>198</v>
       </c>
+      <c r="C200" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="201" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
         <v>199</v>
       </c>
+      <c r="C201" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="202" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
         <v>200</v>
       </c>
+      <c r="C202" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="203" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
@@ -3379,46 +3565,73 @@
       <c r="B204" t="s">
         <v>202</v>
       </c>
+      <c r="C204" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="205" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B205" t="s">
         <v>203</v>
       </c>
+      <c r="C205" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="206" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
         <v>204</v>
       </c>
+      <c r="C206" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="207" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
         <v>205</v>
       </c>
+      <c r="C207" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="208" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
         <v>206</v>
       </c>
+      <c r="C208" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="209" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
         <v>207</v>
       </c>
+      <c r="C209" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="210" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B210" t="s">
         <v>208</v>
       </c>
+      <c r="C210" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="211" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B211" t="s">
         <v>209</v>
       </c>
+      <c r="C211" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="212" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
         <v>210</v>
       </c>
+      <c r="C212" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="213" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B213" t="s">
@@ -3688,6 +3901,9 @@
       <c r="B246" t="s">
         <v>244</v>
       </c>
+      <c r="C246" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="247" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B247" t="s">
@@ -4117,6 +4333,9 @@
       <c r="B300" t="s">
         <v>298</v>
       </c>
+      <c r="D300" t="s">
+        <v>526</v>
+      </c>
     </row>
     <row r="301" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B301" t="s">
@@ -4154,6 +4373,9 @@
       <c r="B305" t="s">
         <v>0</v>
       </c>
+      <c r="C305" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="306" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B306" t="s">
@@ -4863,6 +5085,9 @@
       <c r="B394" t="s">
         <v>391</v>
       </c>
+      <c r="C394" t="s">
+        <v>528</v>
+      </c>
     </row>
     <row r="395" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B395" t="s">
@@ -5119,6 +5344,9 @@
       <c r="B426" t="s">
         <v>423</v>
       </c>
+      <c r="C426" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="427" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B427" t="s">
@@ -5156,6 +5384,9 @@
       <c r="B431" t="s">
         <v>428</v>
       </c>
+      <c r="C431" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="432" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B432" t="s">
@@ -5201,6 +5432,9 @@
       <c r="B437" t="s">
         <v>434</v>
       </c>
+      <c r="C437" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="438" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B438" t="s">
@@ -5262,6 +5496,9 @@
       <c r="B445" t="s">
         <v>442</v>
       </c>
+      <c r="C445" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="446" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B446" t="s">
@@ -5287,7 +5524,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="449" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="449" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B449" t="s">
         <v>446</v>
       </c>
@@ -5295,7 +5532,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="450" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="450" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B450" t="s">
         <v>447</v>
       </c>
@@ -5303,12 +5540,15 @@
         <v>517</v>
       </c>
     </row>
-    <row r="451" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="451" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B451" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="452" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C451" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="452" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B452" t="s">
         <v>449</v>
       </c>
@@ -5316,7 +5556,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="453" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="453" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B453" t="s">
         <v>450</v>
       </c>
@@ -5324,7 +5564,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="454" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="454" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B454" t="s">
         <v>451</v>
       </c>
@@ -5332,7 +5572,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="455" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="455" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B455" t="s">
         <v>452</v>
       </c>
@@ -5340,7 +5580,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="456" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="456" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B456" t="s">
         <v>453</v>
       </c>
@@ -5348,7 +5588,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="457" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="457" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B457" t="s">
         <v>454</v>
       </c>
@@ -5356,15 +5596,15 @@
         <v>517</v>
       </c>
     </row>
-    <row r="458" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="458" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B458" t="s">
         <v>455</v>
       </c>
       <c r="C458" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="459" spans="2:3" x14ac:dyDescent="0.25">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="459" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B459" t="s">
         <v>456</v>
       </c>
@@ -5372,7 +5612,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="460" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="460" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B460" t="s">
         <v>457</v>
       </c>
@@ -5380,15 +5620,18 @@
         <v>517</v>
       </c>
     </row>
-    <row r="461" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="461" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B461" t="s">
         <v>458</v>
       </c>
       <c r="C461" t="s">
+        <v>528</v>
+      </c>
+      <c r="D461" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="462" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="462" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B462" t="s">
         <v>459</v>
       </c>
@@ -5396,7 +5639,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="463" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="463" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B463" t="s">
         <v>460</v>
       </c>
@@ -5404,7 +5647,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="464" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="464" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B464" t="s">
         <v>461</v>
       </c>
@@ -5727,6 +5970,9 @@
     <row r="504" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B504" t="s">
         <v>501</v>
+      </c>
+      <c r="C504" t="s">
+        <v>528</v>
       </c>
       <c r="D504" t="s">
         <v>522</v>

</xml_diff>

<commit_message>
Justin review checklist; relocate people file
</commit_message>
<xml_diff>
--- a/Kate.CheckList.MT.xlsx
+++ b/Kate.CheckList.MT.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3051377\Documents\GitHub\Missionary-Travels\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27729"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10065" windowHeight="7260"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18820" windowHeight="11940"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -24,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="541">
   <si>
     <t>MpÃ©pe (1)</t>
   </si>
@@ -1614,6 +1612,39 @@
   </si>
   <si>
     <t>query</t>
+  </si>
+  <si>
+    <t>add id for Sekote</t>
+  </si>
+  <si>
+    <t>just add id around just 'Moyara'</t>
+  </si>
+  <si>
+    <t>use line 116</t>
+  </si>
+  <si>
+    <t>Leave undefined</t>
+  </si>
+  <si>
+    <t>use id for Monze</t>
+  </si>
+  <si>
+    <t>Use id for Mosilikatise (291)</t>
+  </si>
+  <si>
+    <t>use id for Moyara as above</t>
+  </si>
+  <si>
+    <t>use id for Mozinkwa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> You're correct</t>
+  </si>
+  <si>
+    <t>Use id for Rieg</t>
+  </si>
+  <si>
+    <t>Use Id for Mwant Yav</t>
   </si>
 </sst>
 </file>
@@ -1711,7 +1742,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1746,7 +1777,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1923,7 +1954,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1931,18 +1962,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D518"/>
+  <dimension ref="B2:M518"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="B499" workbookViewId="0">
+      <selection activeCell="G499" sqref="G499"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1950,7 +1981,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -1958,7 +1989,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -1966,7 +1997,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -1974,7 +2005,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -1982,7 +2013,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -1990,7 +2021,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -1998,7 +2029,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -2006,7 +2037,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -2014,7 +2045,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3">
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -2022,7 +2053,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3">
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -2030,7 +2061,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3">
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -2038,7 +2069,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3">
       <c r="B14" t="s">
         <v>12</v>
       </c>
@@ -2046,7 +2077,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:3">
       <c r="B15" t="s">
         <v>13</v>
       </c>
@@ -2054,7 +2085,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:3">
       <c r="B16" t="s">
         <v>14</v>
       </c>
@@ -2062,7 +2093,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3">
       <c r="B17" t="s">
         <v>15</v>
       </c>
@@ -2070,7 +2101,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3">
       <c r="B18" t="s">
         <v>16</v>
       </c>
@@ -2078,7 +2109,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3">
       <c r="B19" t="s">
         <v>17</v>
       </c>
@@ -2086,7 +2117,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3">
       <c r="B20" t="s">
         <v>18</v>
       </c>
@@ -2094,7 +2125,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3">
       <c r="B21" t="s">
         <v>19</v>
       </c>
@@ -2102,7 +2133,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3">
       <c r="B22" t="s">
         <v>20</v>
       </c>
@@ -2110,7 +2141,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3">
       <c r="B23" t="s">
         <v>21</v>
       </c>
@@ -2118,7 +2149,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3">
       <c r="B24" t="s">
         <v>22</v>
       </c>
@@ -2126,7 +2157,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3">
       <c r="B25" t="s">
         <v>23</v>
       </c>
@@ -2134,7 +2165,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3">
       <c r="B26" t="s">
         <v>24</v>
       </c>
@@ -2142,7 +2173,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3">
       <c r="B27" t="s">
         <v>25</v>
       </c>
@@ -2150,7 +2181,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3">
       <c r="B28" t="s">
         <v>26</v>
       </c>
@@ -2158,7 +2189,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3">
       <c r="B29" t="s">
         <v>27</v>
       </c>
@@ -2166,7 +2197,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3">
       <c r="B30" t="s">
         <v>28</v>
       </c>
@@ -2174,7 +2205,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3">
       <c r="B31" t="s">
         <v>29</v>
       </c>
@@ -2182,7 +2213,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3">
       <c r="B32" t="s">
         <v>30</v>
       </c>
@@ -2190,7 +2221,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4">
       <c r="B33" t="s">
         <v>31</v>
       </c>
@@ -2201,7 +2232,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4">
       <c r="B34" t="s">
         <v>32</v>
       </c>
@@ -2209,7 +2240,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4">
       <c r="B35" t="s">
         <v>33</v>
       </c>
@@ -2217,7 +2248,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4">
       <c r="B36" t="s">
         <v>34</v>
       </c>
@@ -2225,7 +2256,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4">
       <c r="B37" t="s">
         <v>35</v>
       </c>
@@ -2233,7 +2264,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4">
       <c r="B38" t="s">
         <v>36</v>
       </c>
@@ -2241,7 +2272,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4">
       <c r="B39" t="s">
         <v>37</v>
       </c>
@@ -2249,7 +2280,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4">
       <c r="B40" t="s">
         <v>38</v>
       </c>
@@ -2257,7 +2288,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4">
       <c r="B41" t="s">
         <v>39</v>
       </c>
@@ -2265,7 +2296,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4">
       <c r="B42" t="s">
         <v>40</v>
       </c>
@@ -2273,7 +2304,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4">
       <c r="B43" t="s">
         <v>41</v>
       </c>
@@ -2281,7 +2312,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4">
       <c r="B44" t="s">
         <v>42</v>
       </c>
@@ -2289,7 +2320,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4">
       <c r="B45" t="s">
         <v>43</v>
       </c>
@@ -2297,7 +2328,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4">
       <c r="B46" t="s">
         <v>44</v>
       </c>
@@ -2305,7 +2336,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4">
       <c r="B47" t="s">
         <v>45</v>
       </c>
@@ -2313,7 +2344,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4">
       <c r="B48" t="s">
         <v>46</v>
       </c>
@@ -2321,7 +2352,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4">
       <c r="B49" t="s">
         <v>47</v>
       </c>
@@ -2329,7 +2360,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4">
       <c r="B50" t="s">
         <v>48</v>
       </c>
@@ -2337,7 +2368,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4">
       <c r="B51" t="s">
         <v>49</v>
       </c>
@@ -2345,7 +2376,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4">
       <c r="B52" t="s">
         <v>50</v>
       </c>
@@ -2353,7 +2384,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4">
       <c r="B53" t="s">
         <v>51</v>
       </c>
@@ -2361,7 +2392,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4">
       <c r="B54" t="s">
         <v>52</v>
       </c>
@@ -2369,7 +2400,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:4">
       <c r="B55" t="s">
         <v>53</v>
       </c>
@@ -2377,7 +2408,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4">
       <c r="B56" t="s">
         <v>54</v>
       </c>
@@ -2385,7 +2416,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4">
       <c r="B57" t="s">
         <v>55</v>
       </c>
@@ -2393,7 +2424,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:4">
       <c r="B58" t="s">
         <v>56</v>
       </c>
@@ -2401,7 +2432,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:4">
       <c r="B59" t="s">
         <v>57</v>
       </c>
@@ -2409,7 +2440,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:4">
       <c r="B60" t="s">
         <v>58</v>
       </c>
@@ -2417,7 +2448,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:4">
       <c r="B61" t="s">
         <v>59</v>
       </c>
@@ -2425,7 +2456,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:4">
       <c r="B62" t="s">
         <v>60</v>
       </c>
@@ -2433,7 +2464,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:4">
       <c r="B63" t="s">
         <v>61</v>
       </c>
@@ -2441,7 +2472,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:4">
       <c r="B64" t="s">
         <v>62</v>
       </c>
@@ -2449,7 +2480,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:3">
       <c r="B65" t="s">
         <v>63</v>
       </c>
@@ -2457,7 +2488,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:3">
       <c r="B66" t="s">
         <v>64</v>
       </c>
@@ -2465,7 +2496,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:3">
       <c r="B67" t="s">
         <v>65</v>
       </c>
@@ -2473,7 +2504,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:3">
       <c r="B68" t="s">
         <v>66</v>
       </c>
@@ -2481,7 +2512,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:3">
       <c r="B69" t="s">
         <v>67</v>
       </c>
@@ -2489,7 +2520,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:3">
       <c r="B70" t="s">
         <v>68</v>
       </c>
@@ -2497,7 +2528,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:3">
       <c r="B71" t="s">
         <v>69</v>
       </c>
@@ -2505,7 +2536,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:3">
       <c r="B72" t="s">
         <v>70</v>
       </c>
@@ -2513,7 +2544,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:3">
       <c r="B73" t="s">
         <v>71</v>
       </c>
@@ -2521,7 +2552,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:3">
       <c r="B74" t="s">
         <v>72</v>
       </c>
@@ -2529,7 +2560,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:3">
       <c r="B75" t="s">
         <v>73</v>
       </c>
@@ -2537,7 +2568,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:3">
       <c r="B76" t="s">
         <v>74</v>
       </c>
@@ -2545,7 +2576,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:3">
       <c r="B77" t="s">
         <v>75</v>
       </c>
@@ -2553,7 +2584,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:3">
       <c r="B78" t="s">
         <v>76</v>
       </c>
@@ -2561,7 +2592,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:3">
       <c r="B79" t="s">
         <v>77</v>
       </c>
@@ -2569,7 +2600,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:3">
       <c r="B80" t="s">
         <v>78</v>
       </c>
@@ -2577,7 +2608,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:3">
       <c r="B81" t="s">
         <v>79</v>
       </c>
@@ -2585,7 +2616,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:3">
       <c r="B82" t="s">
         <v>80</v>
       </c>
@@ -2593,7 +2624,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:3">
       <c r="B83" t="s">
         <v>81</v>
       </c>
@@ -2601,7 +2632,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:3">
       <c r="B84" t="s">
         <v>82</v>
       </c>
@@ -2609,7 +2640,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:3">
       <c r="B85" t="s">
         <v>83</v>
       </c>
@@ -2617,7 +2648,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:3">
       <c r="B86" t="s">
         <v>84</v>
       </c>
@@ -2625,7 +2656,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:3">
       <c r="B87" t="s">
         <v>85</v>
       </c>
@@ -2633,7 +2664,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:3">
       <c r="B88" t="s">
         <v>86</v>
       </c>
@@ -2641,7 +2672,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:3">
       <c r="B89" t="s">
         <v>87</v>
       </c>
@@ -2649,7 +2680,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:3">
       <c r="B90" t="s">
         <v>88</v>
       </c>
@@ -2657,7 +2688,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:3">
       <c r="B91" t="s">
         <v>89</v>
       </c>
@@ -2665,7 +2696,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:3">
       <c r="B92" t="s">
         <v>90</v>
       </c>
@@ -2673,7 +2704,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:3">
       <c r="B93" t="s">
         <v>91</v>
       </c>
@@ -2681,7 +2712,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:3">
       <c r="B94" t="s">
         <v>92</v>
       </c>
@@ -2689,7 +2720,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:3">
       <c r="B95" t="s">
         <v>93</v>
       </c>
@@ -2697,7 +2728,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:3">
       <c r="B96" t="s">
         <v>94</v>
       </c>
@@ -2705,7 +2736,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:4">
       <c r="B97" t="s">
         <v>95</v>
       </c>
@@ -2713,7 +2744,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:4">
       <c r="B98" t="s">
         <v>96</v>
       </c>
@@ -2721,7 +2752,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:4">
       <c r="B99" t="s">
         <v>97</v>
       </c>
@@ -2729,7 +2760,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:4">
       <c r="B100" t="s">
         <v>98</v>
       </c>
@@ -2737,7 +2768,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:4">
       <c r="B101" t="s">
         <v>99</v>
       </c>
@@ -2745,7 +2776,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:4">
       <c r="B102" t="s">
         <v>100</v>
       </c>
@@ -2753,7 +2784,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:4">
       <c r="B103" t="s">
         <v>101</v>
       </c>
@@ -2761,7 +2792,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:4">
       <c r="B104" t="s">
         <v>102</v>
       </c>
@@ -2769,7 +2800,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:4">
       <c r="B105" t="s">
         <v>103</v>
       </c>
@@ -2777,7 +2808,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:4">
       <c r="B106" t="s">
         <v>104</v>
       </c>
@@ -2785,7 +2816,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:4">
       <c r="B107" t="s">
         <v>105</v>
       </c>
@@ -2793,7 +2824,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:4">
       <c r="B108" t="s">
         <v>106</v>
       </c>
@@ -2801,7 +2832,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:4">
       <c r="B109" t="s">
         <v>107</v>
       </c>
@@ -2809,7 +2840,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:4">
       <c r="B110" t="s">
         <v>108</v>
       </c>
@@ -2817,7 +2848,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:4">
       <c r="B111" t="s">
         <v>109</v>
       </c>
@@ -2825,7 +2856,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:4">
       <c r="B112" t="s">
         <v>110</v>
       </c>
@@ -2833,7 +2864,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:5">
       <c r="B113" t="s">
         <v>111</v>
       </c>
@@ -2841,7 +2872,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:5">
       <c r="B114" t="s">
         <v>112</v>
       </c>
@@ -2849,7 +2880,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:5">
       <c r="B115" t="s">
         <v>113</v>
       </c>
@@ -2857,7 +2888,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:5">
       <c r="B116" t="s">
         <v>114</v>
       </c>
@@ -2865,15 +2896,18 @@
         <v>517</v>
       </c>
     </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:5">
       <c r="B117" t="s">
         <v>115</v>
       </c>
       <c r="D117" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E117" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5">
       <c r="B118" t="s">
         <v>116</v>
       </c>
@@ -2881,7 +2915,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:5">
       <c r="B119" t="s">
         <v>117</v>
       </c>
@@ -2889,7 +2923,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:5">
       <c r="B120" t="s">
         <v>118</v>
       </c>
@@ -2897,7 +2931,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:5">
       <c r="B121" t="s">
         <v>119</v>
       </c>
@@ -2905,7 +2939,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:5">
       <c r="B122" t="s">
         <v>120</v>
       </c>
@@ -2913,7 +2947,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:5">
       <c r="B123" t="s">
         <v>121</v>
       </c>
@@ -2921,15 +2955,18 @@
         <v>517</v>
       </c>
     </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:5">
       <c r="B124" t="s">
         <v>122</v>
       </c>
       <c r="D124" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E124" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="125" spans="2:5">
       <c r="B125" t="s">
         <v>123</v>
       </c>
@@ -2937,7 +2974,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:5">
       <c r="B126" t="s">
         <v>124</v>
       </c>
@@ -2945,7 +2982,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:5">
       <c r="B127" t="s">
         <v>125</v>
       </c>
@@ -2953,7 +2990,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:5">
       <c r="B128" t="s">
         <v>126</v>
       </c>
@@ -2961,7 +2998,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:3">
       <c r="B129" t="s">
         <v>127</v>
       </c>
@@ -2969,7 +3006,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:3">
       <c r="B130" t="s">
         <v>128</v>
       </c>
@@ -2977,7 +3014,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:3">
       <c r="B131" t="s">
         <v>129</v>
       </c>
@@ -2985,7 +3022,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:3">
       <c r="B132" t="s">
         <v>130</v>
       </c>
@@ -2993,7 +3030,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:3">
       <c r="B133" t="s">
         <v>131</v>
       </c>
@@ -3001,7 +3038,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:3">
       <c r="B134" t="s">
         <v>132</v>
       </c>
@@ -3009,7 +3046,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:3">
       <c r="B135" t="s">
         <v>133</v>
       </c>
@@ -3017,7 +3054,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:3">
       <c r="B136" t="s">
         <v>134</v>
       </c>
@@ -3025,7 +3062,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:3">
       <c r="B137" t="s">
         <v>135</v>
       </c>
@@ -3033,7 +3070,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:3">
       <c r="B138" t="s">
         <v>136</v>
       </c>
@@ -3041,7 +3078,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:3">
       <c r="B139" t="s">
         <v>137</v>
       </c>
@@ -3049,7 +3086,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:3">
       <c r="B140" t="s">
         <v>138</v>
       </c>
@@ -3057,7 +3094,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:3">
       <c r="B141" t="s">
         <v>139</v>
       </c>
@@ -3065,7 +3102,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:3">
       <c r="B142" t="s">
         <v>140</v>
       </c>
@@ -3073,7 +3110,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:3">
       <c r="B143" t="s">
         <v>141</v>
       </c>
@@ -3081,7 +3118,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:3">
       <c r="B144" t="s">
         <v>142</v>
       </c>
@@ -3089,7 +3126,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:3">
       <c r="B145" t="s">
         <v>143</v>
       </c>
@@ -3097,7 +3134,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:3">
       <c r="B146" t="s">
         <v>144</v>
       </c>
@@ -3105,7 +3142,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:3">
       <c r="B147" t="s">
         <v>145</v>
       </c>
@@ -3113,7 +3150,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:3">
       <c r="B148" t="s">
         <v>146</v>
       </c>
@@ -3121,7 +3158,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:3">
       <c r="B149" t="s">
         <v>147</v>
       </c>
@@ -3129,7 +3166,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:3">
       <c r="B150" t="s">
         <v>148</v>
       </c>
@@ -3137,7 +3174,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:3">
       <c r="B151" t="s">
         <v>149</v>
       </c>
@@ -3145,7 +3182,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:3">
       <c r="B152" t="s">
         <v>150</v>
       </c>
@@ -3153,7 +3190,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="153" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:3">
       <c r="B153" t="s">
         <v>151</v>
       </c>
@@ -3161,7 +3198,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="154" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:3">
       <c r="B154" t="s">
         <v>152</v>
       </c>
@@ -3169,7 +3206,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="155" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:3">
       <c r="B155" t="s">
         <v>153</v>
       </c>
@@ -3177,7 +3214,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="156" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:3">
       <c r="B156" t="s">
         <v>154</v>
       </c>
@@ -3185,7 +3222,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="157" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:3">
       <c r="B157" t="s">
         <v>155</v>
       </c>
@@ -3193,7 +3230,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="158" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:3">
       <c r="B158" t="s">
         <v>156</v>
       </c>
@@ -3201,7 +3238,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="159" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:3">
       <c r="B159" t="s">
         <v>157</v>
       </c>
@@ -3209,7 +3246,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="160" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:3">
       <c r="B160" t="s">
         <v>158</v>
       </c>
@@ -3217,7 +3254,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:5">
       <c r="B161" t="s">
         <v>159</v>
       </c>
@@ -3225,7 +3262,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:5">
       <c r="B162" t="s">
         <v>160</v>
       </c>
@@ -3233,7 +3270,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:5">
       <c r="B163" t="s">
         <v>161</v>
       </c>
@@ -3241,7 +3278,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="164" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:5">
       <c r="B164" t="s">
         <v>162</v>
       </c>
@@ -3249,7 +3286,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:5">
       <c r="B165" t="s">
         <v>163</v>
       </c>
@@ -3257,7 +3294,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:5">
       <c r="B166" t="s">
         <v>164</v>
       </c>
@@ -3265,15 +3302,18 @@
         <v>517</v>
       </c>
     </row>
-    <row r="167" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:5">
       <c r="B167" t="s">
         <v>165</v>
       </c>
       <c r="D167" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="168" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E167" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="168" spans="2:5">
       <c r="B168" t="s">
         <v>166</v>
       </c>
@@ -3281,7 +3321,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="169" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:5">
       <c r="B169" t="s">
         <v>167</v>
       </c>
@@ -3289,7 +3329,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="170" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:5">
       <c r="B170" t="s">
         <v>168</v>
       </c>
@@ -3297,7 +3337,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:5">
       <c r="B171" t="s">
         <v>169</v>
       </c>
@@ -3305,7 +3345,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="172" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:5">
       <c r="B172" t="s">
         <v>170</v>
       </c>
@@ -3313,7 +3353,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:5">
       <c r="B173" t="s">
         <v>171</v>
       </c>
@@ -3321,7 +3361,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="174" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:5">
       <c r="B174" t="s">
         <v>172</v>
       </c>
@@ -3329,7 +3369,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="175" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:5">
       <c r="B175" t="s">
         <v>173</v>
       </c>
@@ -3337,7 +3377,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:5">
       <c r="B176" t="s">
         <v>174</v>
       </c>
@@ -3345,7 +3385,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:5">
       <c r="B177" t="s">
         <v>175</v>
       </c>
@@ -3353,7 +3393,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:5">
       <c r="B178" t="s">
         <v>176</v>
       </c>
@@ -3361,7 +3401,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:5">
       <c r="B179" t="s">
         <v>177</v>
       </c>
@@ -3369,7 +3409,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="180" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:5">
       <c r="B180" t="s">
         <v>178</v>
       </c>
@@ -3377,7 +3417,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:5">
       <c r="B181" t="s">
         <v>179</v>
       </c>
@@ -3385,7 +3425,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:5">
       <c r="B182" t="s">
         <v>180</v>
       </c>
@@ -3393,7 +3433,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="183" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:5">
       <c r="B183" t="s">
         <v>181</v>
       </c>
@@ -3401,7 +3441,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:5">
       <c r="B184" t="s">
         <v>182</v>
       </c>
@@ -3409,7 +3449,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="185" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:5">
       <c r="B185" t="s">
         <v>183</v>
       </c>
@@ -3417,7 +3457,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="186" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:5">
       <c r="B186" t="s">
         <v>184</v>
       </c>
@@ -3425,7 +3465,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="187" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:5">
       <c r="B187" t="s">
         <v>185</v>
       </c>
@@ -3433,7 +3473,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="188" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:5">
       <c r="B188" t="s">
         <v>186</v>
       </c>
@@ -3441,7 +3481,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="189" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:5">
       <c r="B189" t="s">
         <v>187</v>
       </c>
@@ -3449,7 +3489,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="190" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:5">
       <c r="B190" t="s">
         <v>188</v>
       </c>
@@ -3457,15 +3497,18 @@
         <v>517</v>
       </c>
     </row>
-    <row r="191" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:5">
       <c r="B191" t="s">
         <v>189</v>
       </c>
       <c r="D191" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="192" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E191" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="192" spans="2:5">
       <c r="B192" t="s">
         <v>190</v>
       </c>
@@ -3473,7 +3516,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="193" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:3">
       <c r="B193" t="s">
         <v>191</v>
       </c>
@@ -3481,7 +3524,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="194" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:3">
       <c r="B194" t="s">
         <v>192</v>
       </c>
@@ -3489,7 +3532,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="195" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:3">
       <c r="B195" t="s">
         <v>193</v>
       </c>
@@ -3497,7 +3540,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="196" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:3">
       <c r="B196" t="s">
         <v>194</v>
       </c>
@@ -3505,7 +3548,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="197" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:3">
       <c r="B197" t="s">
         <v>195</v>
       </c>
@@ -3513,7 +3556,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="198" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:3">
       <c r="B198" t="s">
         <v>196</v>
       </c>
@@ -3521,7 +3564,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="199" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:3">
       <c r="B199" t="s">
         <v>197</v>
       </c>
@@ -3529,7 +3572,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="200" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:3">
       <c r="B200" t="s">
         <v>198</v>
       </c>
@@ -3537,7 +3580,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="201" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:3">
       <c r="B201" t="s">
         <v>199</v>
       </c>
@@ -3545,7 +3588,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="202" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:3">
       <c r="B202" t="s">
         <v>200</v>
       </c>
@@ -3553,7 +3596,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="203" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:3">
       <c r="B203" t="s">
         <v>201</v>
       </c>
@@ -3561,7 +3604,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="204" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:3">
       <c r="B204" t="s">
         <v>202</v>
       </c>
@@ -3569,7 +3612,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="205" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:3">
       <c r="B205" t="s">
         <v>203</v>
       </c>
@@ -3577,7 +3620,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="206" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:3">
       <c r="B206" t="s">
         <v>204</v>
       </c>
@@ -3585,7 +3628,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="207" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:3">
       <c r="B207" t="s">
         <v>205</v>
       </c>
@@ -3593,7 +3636,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="208" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:3">
       <c r="B208" t="s">
         <v>206</v>
       </c>
@@ -3601,7 +3644,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="209" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:3">
       <c r="B209" t="s">
         <v>207</v>
       </c>
@@ -3609,7 +3652,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="210" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:3">
       <c r="B210" t="s">
         <v>208</v>
       </c>
@@ -3617,7 +3660,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="211" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:3">
       <c r="B211" t="s">
         <v>209</v>
       </c>
@@ -3625,7 +3668,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="212" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:3">
       <c r="B212" t="s">
         <v>210</v>
       </c>
@@ -3633,7 +3676,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="213" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:3">
       <c r="B213" t="s">
         <v>211</v>
       </c>
@@ -3641,7 +3684,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="214" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:3">
       <c r="B214" t="s">
         <v>212</v>
       </c>
@@ -3649,7 +3692,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="215" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:3">
       <c r="B215" t="s">
         <v>213</v>
       </c>
@@ -3657,7 +3700,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="216" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:3">
       <c r="B216" t="s">
         <v>214</v>
       </c>
@@ -3665,7 +3708,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="217" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:3">
       <c r="B217" t="s">
         <v>215</v>
       </c>
@@ -3673,7 +3716,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="218" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:3">
       <c r="B218" t="s">
         <v>216</v>
       </c>
@@ -3681,7 +3724,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="219" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:3">
       <c r="B219" t="s">
         <v>217</v>
       </c>
@@ -3689,7 +3732,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="220" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:3">
       <c r="B220" t="s">
         <v>218</v>
       </c>
@@ -3697,7 +3740,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="221" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:3">
       <c r="B221" t="s">
         <v>219</v>
       </c>
@@ -3705,7 +3748,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="222" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:3">
       <c r="B222" t="s">
         <v>220</v>
       </c>
@@ -3713,7 +3756,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="223" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:3">
       <c r="B223" t="s">
         <v>221</v>
       </c>
@@ -3721,7 +3764,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="224" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:3">
       <c r="B224" t="s">
         <v>222</v>
       </c>
@@ -3729,7 +3772,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="225" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:3">
       <c r="B225" t="s">
         <v>223</v>
       </c>
@@ -3737,7 +3780,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="226" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:3">
       <c r="B226" t="s">
         <v>224</v>
       </c>
@@ -3745,7 +3788,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="227" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:3">
       <c r="B227" t="s">
         <v>225</v>
       </c>
@@ -3753,7 +3796,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="228" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:3">
       <c r="B228" t="s">
         <v>226</v>
       </c>
@@ -3761,7 +3804,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="229" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:3">
       <c r="B229" t="s">
         <v>227</v>
       </c>
@@ -3769,7 +3812,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="230" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:3">
       <c r="B230" t="s">
         <v>228</v>
       </c>
@@ -3777,7 +3820,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="231" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:3">
       <c r="B231" t="s">
         <v>229</v>
       </c>
@@ -3785,7 +3828,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="232" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:3">
       <c r="B232" t="s">
         <v>230</v>
       </c>
@@ -3793,7 +3836,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="233" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:3">
       <c r="B233" t="s">
         <v>231</v>
       </c>
@@ -3801,7 +3844,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="234" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:3">
       <c r="B234" t="s">
         <v>232</v>
       </c>
@@ -3809,7 +3852,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="235" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:3">
       <c r="B235" t="s">
         <v>233</v>
       </c>
@@ -3817,7 +3860,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="236" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:3">
       <c r="B236" t="s">
         <v>234</v>
       </c>
@@ -3825,7 +3868,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="237" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:3">
       <c r="B237" t="s">
         <v>235</v>
       </c>
@@ -3833,7 +3876,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="238" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:3">
       <c r="B238" t="s">
         <v>236</v>
       </c>
@@ -3841,7 +3884,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="239" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:3">
       <c r="B239" t="s">
         <v>237</v>
       </c>
@@ -3849,7 +3892,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="240" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:3">
       <c r="B240" t="s">
         <v>238</v>
       </c>
@@ -3857,7 +3900,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="241" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:3">
       <c r="B241" t="s">
         <v>239</v>
       </c>
@@ -3865,7 +3908,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="242" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:3">
       <c r="B242" t="s">
         <v>240</v>
       </c>
@@ -3873,7 +3916,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="243" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:3">
       <c r="B243" t="s">
         <v>241</v>
       </c>
@@ -3881,7 +3924,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="244" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:3">
       <c r="B244" t="s">
         <v>242</v>
       </c>
@@ -3889,7 +3932,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="245" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:3">
       <c r="B245" t="s">
         <v>243</v>
       </c>
@@ -3897,7 +3940,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="246" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:3">
       <c r="B246" t="s">
         <v>244</v>
       </c>
@@ -3905,7 +3948,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="247" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:3">
       <c r="B247" t="s">
         <v>245</v>
       </c>
@@ -3913,7 +3956,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="248" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:3">
       <c r="B248" t="s">
         <v>246</v>
       </c>
@@ -3921,7 +3964,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="249" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:3">
       <c r="B249" t="s">
         <v>247</v>
       </c>
@@ -3929,7 +3972,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="250" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:3">
       <c r="B250" t="s">
         <v>248</v>
       </c>
@@ -3937,7 +3980,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="251" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:3">
       <c r="B251" t="s">
         <v>249</v>
       </c>
@@ -3945,7 +3988,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="252" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:3">
       <c r="B252" t="s">
         <v>250</v>
       </c>
@@ -3953,7 +3996,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="253" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:3">
       <c r="B253" t="s">
         <v>251</v>
       </c>
@@ -3961,7 +4004,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="254" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="2:3">
       <c r="B254" t="s">
         <v>252</v>
       </c>
@@ -3969,7 +4012,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="255" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="255" spans="2:3">
       <c r="B255" t="s">
         <v>253</v>
       </c>
@@ -3977,7 +4020,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="256" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="2:3">
       <c r="B256" t="s">
         <v>254</v>
       </c>
@@ -3985,7 +4028,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="257" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:3">
       <c r="B257" t="s">
         <v>255</v>
       </c>
@@ -3993,7 +4036,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="258" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:3">
       <c r="B258" t="s">
         <v>256</v>
       </c>
@@ -4001,7 +4044,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="259" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:3">
       <c r="B259" t="s">
         <v>257</v>
       </c>
@@ -4009,7 +4052,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="260" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="260" spans="2:3">
       <c r="B260" t="s">
         <v>258</v>
       </c>
@@ -4017,7 +4060,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="261" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:3">
       <c r="B261" t="s">
         <v>259</v>
       </c>
@@ -4025,7 +4068,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="262" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:3">
       <c r="B262" t="s">
         <v>260</v>
       </c>
@@ -4033,7 +4076,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="263" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:3">
       <c r="B263" t="s">
         <v>261</v>
       </c>
@@ -4041,7 +4084,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="264" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:3">
       <c r="B264" t="s">
         <v>262</v>
       </c>
@@ -4049,7 +4092,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="265" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:3">
       <c r="B265" t="s">
         <v>263</v>
       </c>
@@ -4057,7 +4100,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="266" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:3">
       <c r="B266" t="s">
         <v>264</v>
       </c>
@@ -4065,7 +4108,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="267" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:3">
       <c r="B267" t="s">
         <v>265</v>
       </c>
@@ -4073,7 +4116,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="268" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="268" spans="2:3">
       <c r="B268" t="s">
         <v>266</v>
       </c>
@@ -4081,7 +4124,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="269" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="269" spans="2:3">
       <c r="B269" t="s">
         <v>267</v>
       </c>
@@ -4089,7 +4132,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="270" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="270" spans="2:3">
       <c r="B270" t="s">
         <v>268</v>
       </c>
@@ -4097,7 +4140,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="271" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="271" spans="2:3">
       <c r="B271" t="s">
         <v>269</v>
       </c>
@@ -4105,7 +4148,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="272" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="272" spans="2:3">
       <c r="B272" t="s">
         <v>270</v>
       </c>
@@ -4113,7 +4156,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="273" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="273" spans="2:5">
       <c r="B273" t="s">
         <v>271</v>
       </c>
@@ -4121,15 +4164,18 @@
         <v>517</v>
       </c>
     </row>
-    <row r="274" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="274" spans="2:5">
       <c r="B274" t="s">
         <v>272</v>
       </c>
       <c r="D274" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="275" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E274" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="275" spans="2:5">
       <c r="B275" t="s">
         <v>273</v>
       </c>
@@ -4137,7 +4183,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="276" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="276" spans="2:5">
       <c r="B276" t="s">
         <v>274</v>
       </c>
@@ -4145,7 +4191,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="277" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="277" spans="2:5">
       <c r="B277" t="s">
         <v>275</v>
       </c>
@@ -4153,15 +4199,18 @@
         <v>517</v>
       </c>
     </row>
-    <row r="278" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="278" spans="2:5">
       <c r="B278" t="s">
         <v>276</v>
       </c>
       <c r="D278" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="279" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E278" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="279" spans="2:5">
       <c r="B279" t="s">
         <v>277</v>
       </c>
@@ -4169,7 +4218,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="280" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="280" spans="2:5">
       <c r="B280" t="s">
         <v>278</v>
       </c>
@@ -4177,7 +4226,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="281" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="281" spans="2:5">
       <c r="B281" t="s">
         <v>279</v>
       </c>
@@ -4185,15 +4234,18 @@
         <v>517</v>
       </c>
     </row>
-    <row r="282" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="282" spans="2:5">
       <c r="B282" t="s">
         <v>280</v>
       </c>
       <c r="D282" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="283" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E282" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="283" spans="2:5">
       <c r="B283" t="s">
         <v>281</v>
       </c>
@@ -4201,7 +4253,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="284" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="284" spans="2:5">
       <c r="B284" t="s">
         <v>282</v>
       </c>
@@ -4209,7 +4261,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="285" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="285" spans="2:5">
       <c r="B285" t="s">
         <v>283</v>
       </c>
@@ -4217,7 +4269,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="286" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="286" spans="2:5">
       <c r="B286" t="s">
         <v>284</v>
       </c>
@@ -4225,7 +4277,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="287" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="287" spans="2:5">
       <c r="B287" t="s">
         <v>285</v>
       </c>
@@ -4233,7 +4285,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="288" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="288" spans="2:5">
       <c r="B288" t="s">
         <v>286</v>
       </c>
@@ -4241,15 +4293,18 @@
         <v>517</v>
       </c>
     </row>
-    <row r="289" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="289" spans="2:6">
       <c r="B289" t="s">
         <v>287</v>
       </c>
       <c r="D289" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="290" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E289" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="290" spans="2:6">
       <c r="B290" t="s">
         <v>288</v>
       </c>
@@ -4257,7 +4312,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="291" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="291" spans="2:6">
       <c r="B291" t="s">
         <v>289</v>
       </c>
@@ -4265,7 +4320,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="292" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="292" spans="2:6">
       <c r="B292" t="s">
         <v>290</v>
       </c>
@@ -4273,7 +4328,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="293" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="293" spans="2:6">
       <c r="B293" t="s">
         <v>291</v>
       </c>
@@ -4281,7 +4336,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="294" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="294" spans="2:6">
       <c r="B294" t="s">
         <v>292</v>
       </c>
@@ -4289,7 +4344,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="295" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="295" spans="2:6">
       <c r="B295" t="s">
         <v>293</v>
       </c>
@@ -4297,7 +4352,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="296" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="296" spans="2:6">
       <c r="B296" t="s">
         <v>294</v>
       </c>
@@ -4305,7 +4360,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="297" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="297" spans="2:6">
       <c r="B297" t="s">
         <v>295</v>
       </c>
@@ -4313,7 +4368,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="298" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="298" spans="2:6">
       <c r="B298" t="s">
         <v>296</v>
       </c>
@@ -4321,7 +4376,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="299" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="299" spans="2:6">
       <c r="B299" t="s">
         <v>297</v>
       </c>
@@ -4329,23 +4384,29 @@
         <v>517</v>
       </c>
     </row>
-    <row r="300" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="300" spans="2:6">
       <c r="B300" t="s">
         <v>298</v>
       </c>
       <c r="D300" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="301" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F300" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="301" spans="2:6">
       <c r="B301" t="s">
         <v>299</v>
       </c>
       <c r="D301" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="302" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F301" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="302" spans="2:6">
       <c r="B302" t="s">
         <v>300</v>
       </c>
@@ -4353,7 +4414,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="303" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="303" spans="2:6">
       <c r="B303" t="s">
         <v>301</v>
       </c>
@@ -4361,7 +4422,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="304" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="304" spans="2:6">
       <c r="B304" t="s">
         <v>302</v>
       </c>
@@ -4369,7 +4430,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="305" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="305" spans="2:3">
       <c r="B305" t="s">
         <v>0</v>
       </c>
@@ -4377,7 +4438,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="306" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="306" spans="2:3">
       <c r="B306" t="s">
         <v>303</v>
       </c>
@@ -4385,7 +4446,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="307" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="307" spans="2:3">
       <c r="B307" t="s">
         <v>304</v>
       </c>
@@ -4393,7 +4454,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="308" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="308" spans="2:3">
       <c r="B308" t="s">
         <v>305</v>
       </c>
@@ -4401,7 +4462,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="309" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="309" spans="2:3">
       <c r="B309" t="s">
         <v>306</v>
       </c>
@@ -4409,7 +4470,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="310" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="310" spans="2:3">
       <c r="B310" t="s">
         <v>307</v>
       </c>
@@ -4417,7 +4478,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="311" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="311" spans="2:3">
       <c r="B311" t="s">
         <v>308</v>
       </c>
@@ -4425,7 +4486,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="312" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="312" spans="2:3">
       <c r="B312" t="s">
         <v>309</v>
       </c>
@@ -4433,7 +4494,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="313" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="313" spans="2:3">
       <c r="B313" t="s">
         <v>310</v>
       </c>
@@ -4441,7 +4502,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="314" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="314" spans="2:3">
       <c r="B314" t="s">
         <v>311</v>
       </c>
@@ -4449,7 +4510,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="315" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="315" spans="2:3">
       <c r="B315" t="s">
         <v>312</v>
       </c>
@@ -4457,7 +4518,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="316" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="316" spans="2:3">
       <c r="B316" t="s">
         <v>313</v>
       </c>
@@ -4465,7 +4526,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="317" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="317" spans="2:3">
       <c r="B317" t="s">
         <v>314</v>
       </c>
@@ -4473,7 +4534,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="318" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="318" spans="2:3">
       <c r="B318" t="s">
         <v>315</v>
       </c>
@@ -4481,7 +4542,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="319" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="319" spans="2:3">
       <c r="B319" t="s">
         <v>316</v>
       </c>
@@ -4489,7 +4550,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="320" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="320" spans="2:3">
       <c r="B320" t="s">
         <v>317</v>
       </c>
@@ -4497,7 +4558,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="321" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="321" spans="2:3">
       <c r="B321" t="s">
         <v>318</v>
       </c>
@@ -4505,7 +4566,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="322" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="322" spans="2:3">
       <c r="B322" t="s">
         <v>319</v>
       </c>
@@ -4513,7 +4574,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="323" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="323" spans="2:3">
       <c r="B323" t="s">
         <v>320</v>
       </c>
@@ -4521,7 +4582,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="324" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="324" spans="2:3">
       <c r="B324" t="s">
         <v>321</v>
       </c>
@@ -4529,7 +4590,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="325" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="325" spans="2:3">
       <c r="B325" t="s">
         <v>322</v>
       </c>
@@ -4537,7 +4598,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="326" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="326" spans="2:3">
       <c r="B326" t="s">
         <v>323</v>
       </c>
@@ -4545,7 +4606,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="327" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="327" spans="2:3">
       <c r="B327" t="s">
         <v>324</v>
       </c>
@@ -4553,7 +4614,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="328" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="328" spans="2:3">
       <c r="B328" t="s">
         <v>325</v>
       </c>
@@ -4561,7 +4622,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="329" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="329" spans="2:3">
       <c r="B329" t="s">
         <v>326</v>
       </c>
@@ -4569,7 +4630,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="330" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="330" spans="2:3">
       <c r="B330" t="s">
         <v>327</v>
       </c>
@@ -4577,7 +4638,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="331" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="331" spans="2:3">
       <c r="B331" t="s">
         <v>328</v>
       </c>
@@ -4585,7 +4646,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="332" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="332" spans="2:3">
       <c r="B332" t="s">
         <v>329</v>
       </c>
@@ -4593,7 +4654,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="333" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="333" spans="2:3">
       <c r="B333" t="s">
         <v>330</v>
       </c>
@@ -4601,7 +4662,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="334" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="334" spans="2:3">
       <c r="B334" t="s">
         <v>331</v>
       </c>
@@ -4609,7 +4670,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="335" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="335" spans="2:3">
       <c r="B335" t="s">
         <v>332</v>
       </c>
@@ -4617,7 +4678,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="336" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="336" spans="2:3">
       <c r="B336" t="s">
         <v>333</v>
       </c>
@@ -4625,7 +4686,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="337" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="337" spans="2:13">
       <c r="B337" t="s">
         <v>334</v>
       </c>
@@ -4633,7 +4694,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="338" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="338" spans="2:13">
       <c r="B338" t="s">
         <v>335</v>
       </c>
@@ -4641,7 +4702,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="339" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="339" spans="2:13">
       <c r="B339" t="s">
         <v>336</v>
       </c>
@@ -4649,7 +4710,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="340" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="340" spans="2:13">
       <c r="B340" t="s">
         <v>337</v>
       </c>
@@ -4657,7 +4718,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="341" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="341" spans="2:13">
       <c r="B341" t="s">
         <v>338</v>
       </c>
@@ -4665,7 +4726,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="342" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="342" spans="2:13">
       <c r="B342" t="s">
         <v>339</v>
       </c>
@@ -4673,7 +4734,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="343" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="343" spans="2:13">
       <c r="B343" t="s">
         <v>340</v>
       </c>
@@ -4681,7 +4742,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="344" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="344" spans="2:13">
       <c r="B344" t="s">
         <v>341</v>
       </c>
@@ -4689,7 +4750,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="345" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="345" spans="2:13">
       <c r="B345" t="s">
         <v>342</v>
       </c>
@@ -4697,7 +4758,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="346" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="346" spans="2:13">
       <c r="B346" t="s">
         <v>343</v>
       </c>
@@ -4705,15 +4766,18 @@
         <v>517</v>
       </c>
     </row>
-    <row r="347" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="347" spans="2:13">
       <c r="B347" t="s">
         <v>344</v>
       </c>
       <c r="D347" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="348" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="M347" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="348" spans="2:13">
       <c r="B348" t="s">
         <v>345</v>
       </c>
@@ -4721,7 +4785,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="349" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="349" spans="2:13">
       <c r="B349" t="s">
         <v>346</v>
       </c>
@@ -4729,7 +4793,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="350" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="350" spans="2:13">
       <c r="B350" t="s">
         <v>347</v>
       </c>
@@ -4737,7 +4801,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="351" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="351" spans="2:13">
       <c r="B351" t="s">
         <v>348</v>
       </c>
@@ -4745,7 +4809,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="352" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="352" spans="2:13">
       <c r="B352" t="s">
         <v>349</v>
       </c>
@@ -4753,7 +4817,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="353" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="353" spans="2:9">
       <c r="B353" t="s">
         <v>350</v>
       </c>
@@ -4761,7 +4825,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="354" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="354" spans="2:9">
       <c r="B354" t="s">
         <v>351</v>
       </c>
@@ -4769,7 +4833,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="355" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="355" spans="2:9">
       <c r="B355" t="s">
         <v>352</v>
       </c>
@@ -4777,7 +4841,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="356" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="356" spans="2:9">
       <c r="B356" t="s">
         <v>353</v>
       </c>
@@ -4785,7 +4849,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="357" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="357" spans="2:9">
       <c r="B357" t="s">
         <v>354</v>
       </c>
@@ -4793,15 +4857,18 @@
         <v>517</v>
       </c>
     </row>
-    <row r="358" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="358" spans="2:9">
       <c r="B358" t="s">
         <v>355</v>
       </c>
       <c r="D358" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="359" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="I358" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="359" spans="2:9">
       <c r="B359" t="s">
         <v>356</v>
       </c>
@@ -4809,7 +4876,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="360" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="360" spans="2:9">
       <c r="B360" t="s">
         <v>357</v>
       </c>
@@ -4817,7 +4884,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="361" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="361" spans="2:9">
       <c r="B361" t="s">
         <v>358</v>
       </c>
@@ -4825,7 +4892,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="362" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="362" spans="2:9">
       <c r="B362" t="s">
         <v>359</v>
       </c>
@@ -4833,7 +4900,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="363" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="363" spans="2:9">
       <c r="B363" t="s">
         <v>360</v>
       </c>
@@ -4841,7 +4908,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="364" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="364" spans="2:9">
       <c r="B364" t="s">
         <v>361</v>
       </c>
@@ -4849,7 +4916,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="365" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="365" spans="2:9">
       <c r="B365" t="s">
         <v>362</v>
       </c>
@@ -4857,7 +4924,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="366" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="366" spans="2:9">
       <c r="B366" t="s">
         <v>363</v>
       </c>
@@ -4865,7 +4932,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="367" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="367" spans="2:9">
       <c r="B367" t="s">
         <v>364</v>
       </c>
@@ -4873,7 +4940,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="368" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="368" spans="2:9">
       <c r="B368" t="s">
         <v>365</v>
       </c>
@@ -4881,7 +4948,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="369" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="369" spans="2:3">
       <c r="B369" t="s">
         <v>366</v>
       </c>
@@ -4889,7 +4956,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="370" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="370" spans="2:3">
       <c r="B370" t="s">
         <v>367</v>
       </c>
@@ -4897,7 +4964,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="371" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="371" spans="2:3">
       <c r="B371" t="s">
         <v>368</v>
       </c>
@@ -4905,7 +4972,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="372" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="372" spans="2:3">
       <c r="B372" t="s">
         <v>369</v>
       </c>
@@ -4913,7 +4980,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="373" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="373" spans="2:3">
       <c r="B373" t="s">
         <v>370</v>
       </c>
@@ -4921,7 +4988,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="374" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="374" spans="2:3">
       <c r="B374" t="s">
         <v>371</v>
       </c>
@@ -4929,7 +4996,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="375" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="375" spans="2:3">
       <c r="B375" t="s">
         <v>372</v>
       </c>
@@ -4937,7 +5004,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="376" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="376" spans="2:3">
       <c r="B376" t="s">
         <v>373</v>
       </c>
@@ -4945,7 +5012,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="377" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="377" spans="2:3">
       <c r="B377" t="s">
         <v>374</v>
       </c>
@@ -4953,7 +5020,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="378" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="378" spans="2:3">
       <c r="B378" t="s">
         <v>375</v>
       </c>
@@ -4961,7 +5028,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="379" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="379" spans="2:3">
       <c r="B379" t="s">
         <v>376</v>
       </c>
@@ -4969,7 +5036,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="380" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="380" spans="2:3">
       <c r="B380" t="s">
         <v>377</v>
       </c>
@@ -4977,7 +5044,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="381" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="381" spans="2:3">
       <c r="B381" t="s">
         <v>378</v>
       </c>
@@ -4985,7 +5052,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="382" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="382" spans="2:3">
       <c r="B382" t="s">
         <v>379</v>
       </c>
@@ -4993,7 +5060,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="383" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="383" spans="2:3">
       <c r="B383" t="s">
         <v>380</v>
       </c>
@@ -5001,7 +5068,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="384" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="384" spans="2:3">
       <c r="B384" t="s">
         <v>381</v>
       </c>
@@ -5009,7 +5076,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="385" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="385" spans="2:3">
       <c r="B385" t="s">
         <v>382</v>
       </c>
@@ -5017,7 +5084,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="386" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="386" spans="2:3">
       <c r="B386" t="s">
         <v>383</v>
       </c>
@@ -5025,7 +5092,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="387" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="387" spans="2:3">
       <c r="B387" t="s">
         <v>384</v>
       </c>
@@ -5033,7 +5100,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="388" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="388" spans="2:3">
       <c r="B388" t="s">
         <v>385</v>
       </c>
@@ -5041,7 +5108,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="389" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="389" spans="2:3">
       <c r="B389" t="s">
         <v>386</v>
       </c>
@@ -5049,7 +5116,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="390" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="390" spans="2:3">
       <c r="B390" t="s">
         <v>387</v>
       </c>
@@ -5057,7 +5124,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="391" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="391" spans="2:3">
       <c r="B391" t="s">
         <v>388</v>
       </c>
@@ -5065,7 +5132,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="392" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="392" spans="2:3">
       <c r="B392" t="s">
         <v>389</v>
       </c>
@@ -5073,7 +5140,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="393" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="393" spans="2:3">
       <c r="B393" t="s">
         <v>390</v>
       </c>
@@ -5081,7 +5148,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="394" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="394" spans="2:3">
       <c r="B394" t="s">
         <v>391</v>
       </c>
@@ -5089,7 +5156,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="395" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="395" spans="2:3">
       <c r="B395" t="s">
         <v>392</v>
       </c>
@@ -5097,7 +5164,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="396" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="396" spans="2:3">
       <c r="B396" t="s">
         <v>393</v>
       </c>
@@ -5105,7 +5172,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="397" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="397" spans="2:3">
       <c r="B397" t="s">
         <v>394</v>
       </c>
@@ -5113,7 +5180,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="398" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="398" spans="2:3">
       <c r="B398" t="s">
         <v>395</v>
       </c>
@@ -5121,7 +5188,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="399" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="399" spans="2:3">
       <c r="B399" t="s">
         <v>396</v>
       </c>
@@ -5129,7 +5196,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="400" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="400" spans="2:3">
       <c r="B400" t="s">
         <v>397</v>
       </c>
@@ -5137,7 +5204,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="401" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="401" spans="2:7">
       <c r="B401" t="s">
         <v>398</v>
       </c>
@@ -5145,7 +5212,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="402" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="402" spans="2:7">
       <c r="B402" t="s">
         <v>399</v>
       </c>
@@ -5153,7 +5220,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="403" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="403" spans="2:7">
       <c r="B403" t="s">
         <v>400</v>
       </c>
@@ -5161,7 +5228,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="404" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="404" spans="2:7">
       <c r="B404" t="s">
         <v>401</v>
       </c>
@@ -5169,7 +5236,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="405" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="405" spans="2:7">
       <c r="B405" t="s">
         <v>402</v>
       </c>
@@ -5177,7 +5244,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="406" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="406" spans="2:7">
       <c r="B406" t="s">
         <v>403</v>
       </c>
@@ -5185,7 +5252,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="407" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="407" spans="2:7">
       <c r="B407" t="s">
         <v>404</v>
       </c>
@@ -5193,7 +5260,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="408" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="408" spans="2:7">
       <c r="B408" t="s">
         <v>405</v>
       </c>
@@ -5201,7 +5268,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="409" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="409" spans="2:7">
       <c r="B409" t="s">
         <v>406</v>
       </c>
@@ -5209,7 +5276,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="410" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="410" spans="2:7">
       <c r="B410" t="s">
         <v>407</v>
       </c>
@@ -5217,7 +5284,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="411" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="411" spans="2:7">
       <c r="B411" t="s">
         <v>408</v>
       </c>
@@ -5225,7 +5292,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="412" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="412" spans="2:7">
       <c r="B412" t="s">
         <v>409</v>
       </c>
@@ -5233,7 +5300,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="413" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="413" spans="2:7">
       <c r="B413" t="s">
         <v>410</v>
       </c>
@@ -5243,8 +5310,11 @@
       <c r="D413" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="414" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="G413" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="414" spans="2:7">
       <c r="B414" t="s">
         <v>411</v>
       </c>
@@ -5252,7 +5322,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="415" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="415" spans="2:7">
       <c r="B415" t="s">
         <v>412</v>
       </c>
@@ -5260,7 +5330,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="416" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="416" spans="2:7">
       <c r="B416" t="s">
         <v>413</v>
       </c>
@@ -5268,7 +5338,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="417" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="417" spans="2:3">
       <c r="B417" t="s">
         <v>414</v>
       </c>
@@ -5276,7 +5346,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="418" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="418" spans="2:3">
       <c r="B418" t="s">
         <v>415</v>
       </c>
@@ -5284,7 +5354,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="419" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="419" spans="2:3">
       <c r="B419" t="s">
         <v>416</v>
       </c>
@@ -5292,7 +5362,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="420" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="420" spans="2:3">
       <c r="B420" t="s">
         <v>417</v>
       </c>
@@ -5300,7 +5370,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="421" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="421" spans="2:3">
       <c r="B421" t="s">
         <v>418</v>
       </c>
@@ -5308,7 +5378,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="422" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="422" spans="2:3">
       <c r="B422" t="s">
         <v>419</v>
       </c>
@@ -5316,7 +5386,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="423" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="423" spans="2:3">
       <c r="B423" t="s">
         <v>420</v>
       </c>
@@ -5324,7 +5394,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="424" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="424" spans="2:3">
       <c r="B424" t="s">
         <v>421</v>
       </c>
@@ -5332,7 +5402,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="425" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="425" spans="2:3">
       <c r="B425" t="s">
         <v>422</v>
       </c>
@@ -5340,7 +5410,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="426" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="426" spans="2:3">
       <c r="B426" t="s">
         <v>423</v>
       </c>
@@ -5348,7 +5418,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="427" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="427" spans="2:3">
       <c r="B427" t="s">
         <v>424</v>
       </c>
@@ -5356,7 +5426,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="428" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="428" spans="2:3">
       <c r="B428" t="s">
         <v>425</v>
       </c>
@@ -5364,7 +5434,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="429" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="429" spans="2:3">
       <c r="B429" t="s">
         <v>426</v>
       </c>
@@ -5372,7 +5442,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="430" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="430" spans="2:3">
       <c r="B430" t="s">
         <v>427</v>
       </c>
@@ -5380,7 +5450,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="431" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="431" spans="2:3">
       <c r="B431" t="s">
         <v>428</v>
       </c>
@@ -5388,7 +5458,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="432" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="432" spans="2:3">
       <c r="B432" t="s">
         <v>429</v>
       </c>
@@ -5396,7 +5466,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="433" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="433" spans="2:3">
       <c r="B433" t="s">
         <v>430</v>
       </c>
@@ -5404,7 +5474,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="434" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="434" spans="2:3">
       <c r="B434" t="s">
         <v>431</v>
       </c>
@@ -5412,7 +5482,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="435" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="435" spans="2:3">
       <c r="B435" t="s">
         <v>432</v>
       </c>
@@ -5420,7 +5490,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="436" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="436" spans="2:3">
       <c r="B436" t="s">
         <v>433</v>
       </c>
@@ -5428,7 +5498,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="437" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="437" spans="2:3">
       <c r="B437" t="s">
         <v>434</v>
       </c>
@@ -5436,7 +5506,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="438" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="438" spans="2:3">
       <c r="B438" t="s">
         <v>435</v>
       </c>
@@ -5444,7 +5514,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="439" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="439" spans="2:3">
       <c r="B439" t="s">
         <v>436</v>
       </c>
@@ -5452,7 +5522,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="440" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="440" spans="2:3">
       <c r="B440" t="s">
         <v>437</v>
       </c>
@@ -5460,7 +5530,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="441" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="441" spans="2:3">
       <c r="B441" t="s">
         <v>438</v>
       </c>
@@ -5468,7 +5538,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="442" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="442" spans="2:3">
       <c r="B442" t="s">
         <v>439</v>
       </c>
@@ -5476,7 +5546,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="443" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="443" spans="2:3">
       <c r="B443" t="s">
         <v>440</v>
       </c>
@@ -5484,7 +5554,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="444" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="444" spans="2:3">
       <c r="B444" t="s">
         <v>441</v>
       </c>
@@ -5492,7 +5562,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="445" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="445" spans="2:3">
       <c r="B445" t="s">
         <v>442</v>
       </c>
@@ -5500,7 +5570,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="446" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="446" spans="2:3">
       <c r="B446" t="s">
         <v>443</v>
       </c>
@@ -5508,7 +5578,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="447" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="447" spans="2:3">
       <c r="B447" t="s">
         <v>444</v>
       </c>
@@ -5516,7 +5586,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="448" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="448" spans="2:3">
       <c r="B448" t="s">
         <v>445</v>
       </c>
@@ -5524,7 +5594,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="449" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="449" spans="2:4">
       <c r="B449" t="s">
         <v>446</v>
       </c>
@@ -5532,7 +5602,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="450" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="450" spans="2:4">
       <c r="B450" t="s">
         <v>447</v>
       </c>
@@ -5540,7 +5610,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="451" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="451" spans="2:4">
       <c r="B451" t="s">
         <v>448</v>
       </c>
@@ -5548,7 +5618,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="452" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="452" spans="2:4">
       <c r="B452" t="s">
         <v>449</v>
       </c>
@@ -5556,7 +5626,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="453" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="453" spans="2:4">
       <c r="B453" t="s">
         <v>450</v>
       </c>
@@ -5564,7 +5634,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="454" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="454" spans="2:4">
       <c r="B454" t="s">
         <v>451</v>
       </c>
@@ -5572,7 +5642,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="455" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="455" spans="2:4">
       <c r="B455" t="s">
         <v>452</v>
       </c>
@@ -5580,7 +5650,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="456" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="456" spans="2:4">
       <c r="B456" t="s">
         <v>453</v>
       </c>
@@ -5588,7 +5658,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="457" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="457" spans="2:4">
       <c r="B457" t="s">
         <v>454</v>
       </c>
@@ -5596,7 +5666,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="458" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="458" spans="2:4">
       <c r="B458" t="s">
         <v>455</v>
       </c>
@@ -5604,7 +5674,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="459" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="459" spans="2:4">
       <c r="B459" t="s">
         <v>456</v>
       </c>
@@ -5612,7 +5682,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="460" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="460" spans="2:4">
       <c r="B460" t="s">
         <v>457</v>
       </c>
@@ -5620,7 +5690,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="461" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="461" spans="2:4">
       <c r="B461" t="s">
         <v>458</v>
       </c>
@@ -5631,7 +5701,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="462" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="462" spans="2:4">
       <c r="B462" t="s">
         <v>459</v>
       </c>
@@ -5639,7 +5709,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="463" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="463" spans="2:4">
       <c r="B463" t="s">
         <v>460</v>
       </c>
@@ -5647,7 +5717,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="464" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="464" spans="2:4">
       <c r="B464" t="s">
         <v>461</v>
       </c>
@@ -5655,7 +5725,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="465" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="465" spans="2:3">
       <c r="B465" t="s">
         <v>462</v>
       </c>
@@ -5663,7 +5733,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="466" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="466" spans="2:3">
       <c r="B466" t="s">
         <v>463</v>
       </c>
@@ -5671,7 +5741,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="467" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="467" spans="2:3">
       <c r="B467" t="s">
         <v>464</v>
       </c>
@@ -5679,7 +5749,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="468" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="468" spans="2:3">
       <c r="B468" t="s">
         <v>465</v>
       </c>
@@ -5687,7 +5757,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="469" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="469" spans="2:3">
       <c r="B469" t="s">
         <v>466</v>
       </c>
@@ -5695,7 +5765,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="470" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="470" spans="2:3">
       <c r="B470" t="s">
         <v>467</v>
       </c>
@@ -5703,7 +5773,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="471" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="471" spans="2:3">
       <c r="B471" t="s">
         <v>468</v>
       </c>
@@ -5711,7 +5781,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="472" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="472" spans="2:3">
       <c r="B472" t="s">
         <v>469</v>
       </c>
@@ -5719,7 +5789,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="473" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="473" spans="2:3">
       <c r="B473" t="s">
         <v>470</v>
       </c>
@@ -5727,7 +5797,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="474" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="474" spans="2:3">
       <c r="B474" t="s">
         <v>471</v>
       </c>
@@ -5735,7 +5805,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="475" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="475" spans="2:3">
       <c r="B475" t="s">
         <v>472</v>
       </c>
@@ -5743,7 +5813,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="476" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="476" spans="2:3">
       <c r="B476" t="s">
         <v>473</v>
       </c>
@@ -5751,7 +5821,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="477" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="477" spans="2:3">
       <c r="B477" t="s">
         <v>474</v>
       </c>
@@ -5759,7 +5829,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="478" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="478" spans="2:3">
       <c r="B478" t="s">
         <v>475</v>
       </c>
@@ -5767,7 +5837,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="479" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="479" spans="2:3">
       <c r="B479" t="s">
         <v>476</v>
       </c>
@@ -5775,7 +5845,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="480" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="480" spans="2:3">
       <c r="B480" t="s">
         <v>477</v>
       </c>
@@ -5783,7 +5853,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="481" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="481" spans="2:3">
       <c r="B481" t="s">
         <v>478</v>
       </c>
@@ -5791,7 +5861,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="482" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="482" spans="2:3">
       <c r="B482" t="s">
         <v>479</v>
       </c>
@@ -5799,7 +5869,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="483" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="483" spans="2:3">
       <c r="B483" t="s">
         <v>480</v>
       </c>
@@ -5807,7 +5877,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="484" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="484" spans="2:3">
       <c r="B484" t="s">
         <v>481</v>
       </c>
@@ -5815,7 +5885,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="485" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="485" spans="2:3">
       <c r="B485" t="s">
         <v>482</v>
       </c>
@@ -5823,7 +5893,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="486" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="486" spans="2:3">
       <c r="B486" t="s">
         <v>483</v>
       </c>
@@ -5831,7 +5901,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="487" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="487" spans="2:3">
       <c r="B487" t="s">
         <v>484</v>
       </c>
@@ -5839,7 +5909,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="488" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="488" spans="2:3">
       <c r="B488" t="s">
         <v>485</v>
       </c>
@@ -5847,7 +5917,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="489" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="489" spans="2:3">
       <c r="B489" t="s">
         <v>486</v>
       </c>
@@ -5855,7 +5925,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="490" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="490" spans="2:3">
       <c r="B490" t="s">
         <v>487</v>
       </c>
@@ -5863,7 +5933,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="491" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="491" spans="2:3">
       <c r="B491" t="s">
         <v>488</v>
       </c>
@@ -5871,7 +5941,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="492" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="492" spans="2:3">
       <c r="B492" t="s">
         <v>489</v>
       </c>
@@ -5879,7 +5949,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="493" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="493" spans="2:3">
       <c r="B493" t="s">
         <v>490</v>
       </c>
@@ -5887,7 +5957,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="494" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="494" spans="2:3">
       <c r="B494" t="s">
         <v>491</v>
       </c>
@@ -5895,7 +5965,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="495" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="495" spans="2:3">
       <c r="B495" t="s">
         <v>492</v>
       </c>
@@ -5903,7 +5973,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="496" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="496" spans="2:3">
       <c r="B496" t="s">
         <v>493</v>
       </c>
@@ -5911,7 +5981,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="497" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="497" spans="2:4">
       <c r="B497" t="s">
         <v>494</v>
       </c>
@@ -5919,7 +5989,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="498" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="498" spans="2:4">
       <c r="B498" t="s">
         <v>495</v>
       </c>
@@ -5927,7 +5997,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="499" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="499" spans="2:4">
       <c r="B499" t="s">
         <v>496</v>
       </c>
@@ -5935,7 +6005,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="500" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="500" spans="2:4">
       <c r="B500" t="s">
         <v>497</v>
       </c>
@@ -5943,7 +6013,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="501" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="501" spans="2:4">
       <c r="B501" t="s">
         <v>498</v>
       </c>
@@ -5951,7 +6021,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="502" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="502" spans="2:4">
       <c r="B502" t="s">
         <v>499</v>
       </c>
@@ -5959,7 +6029,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="503" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="503" spans="2:4">
       <c r="B503" t="s">
         <v>500</v>
       </c>
@@ -5967,7 +6037,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="504" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="504" spans="2:4">
       <c r="B504" t="s">
         <v>501</v>
       </c>
@@ -5978,7 +6048,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="505" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="505" spans="2:4">
       <c r="B505" t="s">
         <v>502</v>
       </c>
@@ -5986,7 +6056,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="506" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="506" spans="2:4">
       <c r="B506" t="s">
         <v>503</v>
       </c>
@@ -5994,7 +6064,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="507" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="507" spans="2:4">
       <c r="B507" t="s">
         <v>504</v>
       </c>
@@ -6002,7 +6072,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="508" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="508" spans="2:4">
       <c r="B508" t="s">
         <v>505</v>
       </c>
@@ -6010,7 +6080,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="509" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="509" spans="2:4">
       <c r="B509" t="s">
         <v>506</v>
       </c>
@@ -6018,7 +6088,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="510" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="510" spans="2:4">
       <c r="B510" t="s">
         <v>507</v>
       </c>
@@ -6026,7 +6096,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="511" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="511" spans="2:4">
       <c r="B511" t="s">
         <v>508</v>
       </c>
@@ -6034,7 +6104,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="512" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="512" spans="2:4">
       <c r="B512" t="s">
         <v>509</v>
       </c>
@@ -6042,7 +6112,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="513" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="513" spans="2:3">
       <c r="B513" t="s">
         <v>510</v>
       </c>
@@ -6050,7 +6120,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="514" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="514" spans="2:3">
       <c r="B514" t="s">
         <v>511</v>
       </c>
@@ -6058,7 +6128,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="515" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="515" spans="2:3">
       <c r="B515" t="s">
         <v>512</v>
       </c>
@@ -6066,7 +6136,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="516" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="516" spans="2:3">
       <c r="B516" t="s">
         <v>513</v>
       </c>
@@ -6074,7 +6144,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="517" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="517" spans="2:3">
       <c r="B517" t="s">
         <v>514</v>
       </c>
@@ -6082,7 +6152,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="518" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="518" spans="2:3">
       <c r="B518" t="s">
         <v>515</v>
       </c>
@@ -6092,5 +6162,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final amendments to persName id tag
</commit_message>
<xml_diff>
--- a/Kate.CheckList.MT.xlsx
+++ b/Kate.CheckList.MT.xlsx
@@ -1,28 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3051377\Documents\GitHub\Missionary-Travels\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18820" windowHeight="11940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18825" windowHeight="11940"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="541">
   <si>
     <t>MpÃ©pe (1)</t>
   </si>
@@ -1954,7 +1959,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1964,16 +1969,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M518"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B499" workbookViewId="0">
-      <selection activeCell="G499" sqref="G499"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="45.6640625" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1981,7 +1986,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -1989,7 +1994,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -1997,7 +2002,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -2005,7 +2010,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -2013,7 +2018,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -2021,7 +2026,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -2029,7 +2034,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -2037,7 +2042,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -2045,7 +2050,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -2053,7 +2058,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="12" spans="2:3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -2061,7 +2066,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="13" spans="2:3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -2069,7 +2074,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="14" spans="2:3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>12</v>
       </c>
@@ -2077,7 +2082,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>13</v>
       </c>
@@ -2085,7 +2090,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="16" spans="2:3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>14</v>
       </c>
@@ -2093,7 +2098,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>15</v>
       </c>
@@ -2101,7 +2106,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>16</v>
       </c>
@@ -2109,7 +2114,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>17</v>
       </c>
@@ -2117,7 +2122,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>18</v>
       </c>
@@ -2125,7 +2130,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>19</v>
       </c>
@@ -2133,7 +2138,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>20</v>
       </c>
@@ -2141,7 +2146,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>21</v>
       </c>
@@ -2149,7 +2154,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>22</v>
       </c>
@@ -2157,7 +2162,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>23</v>
       </c>
@@ -2165,7 +2170,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="26" spans="2:3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>24</v>
       </c>
@@ -2173,7 +2178,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="27" spans="2:3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>25</v>
       </c>
@@ -2181,7 +2186,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="28" spans="2:3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>26</v>
       </c>
@@ -2189,7 +2194,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="29" spans="2:3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>27</v>
       </c>
@@ -2197,7 +2202,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="30" spans="2:3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>28</v>
       </c>
@@ -2205,7 +2210,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="31" spans="2:3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>29</v>
       </c>
@@ -2213,7 +2218,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="32" spans="2:3">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>30</v>
       </c>
@@ -2221,7 +2226,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="33" spans="2:4">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>31</v>
       </c>
@@ -2232,7 +2237,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="34" spans="2:4">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>32</v>
       </c>
@@ -2240,7 +2245,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="35" spans="2:4">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>33</v>
       </c>
@@ -2248,7 +2253,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="36" spans="2:4">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>34</v>
       </c>
@@ -2256,7 +2261,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="37" spans="2:4">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>35</v>
       </c>
@@ -2264,7 +2269,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="38" spans="2:4">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>36</v>
       </c>
@@ -2272,7 +2277,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="39" spans="2:4">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>37</v>
       </c>
@@ -2280,7 +2285,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="40" spans="2:4">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>38</v>
       </c>
@@ -2288,7 +2293,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="41" spans="2:4">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>39</v>
       </c>
@@ -2296,7 +2301,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="42" spans="2:4">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>40</v>
       </c>
@@ -2304,7 +2309,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="43" spans="2:4">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>41</v>
       </c>
@@ -2312,7 +2317,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="44" spans="2:4">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>42</v>
       </c>
@@ -2320,7 +2325,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="45" spans="2:4">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>43</v>
       </c>
@@ -2328,7 +2333,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="46" spans="2:4">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>44</v>
       </c>
@@ -2336,7 +2341,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="47" spans="2:4">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>45</v>
       </c>
@@ -2344,7 +2349,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="48" spans="2:4">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>46</v>
       </c>
@@ -2352,7 +2357,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="49" spans="2:4">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>47</v>
       </c>
@@ -2360,7 +2365,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="50" spans="2:4">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>48</v>
       </c>
@@ -2368,7 +2373,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="51" spans="2:4">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>49</v>
       </c>
@@ -2376,7 +2381,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="52" spans="2:4">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>50</v>
       </c>
@@ -2384,7 +2389,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="53" spans="2:4">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>51</v>
       </c>
@@ -2392,7 +2397,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="54" spans="2:4">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>52</v>
       </c>
@@ -2400,7 +2405,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="55" spans="2:4">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>53</v>
       </c>
@@ -2408,7 +2413,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="56" spans="2:4">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>54</v>
       </c>
@@ -2416,7 +2421,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="57" spans="2:4">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>55</v>
       </c>
@@ -2424,7 +2429,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="58" spans="2:4">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>56</v>
       </c>
@@ -2432,7 +2437,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="59" spans="2:4">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>57</v>
       </c>
@@ -2440,7 +2445,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="60" spans="2:4">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>58</v>
       </c>
@@ -2448,7 +2453,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="61" spans="2:4">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>59</v>
       </c>
@@ -2456,15 +2461,18 @@
         <v>517</v>
       </c>
     </row>
-    <row r="62" spans="2:4">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>60</v>
       </c>
+      <c r="C62" t="s">
+        <v>517</v>
+      </c>
       <c r="D62" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="63" spans="2:4">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>61</v>
       </c>
@@ -2472,7 +2480,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="64" spans="2:4">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>62</v>
       </c>
@@ -2480,7 +2488,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="65" spans="2:3">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>63</v>
       </c>
@@ -2488,7 +2496,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="66" spans="2:3">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>64</v>
       </c>
@@ -2496,7 +2504,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="67" spans="2:3">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>65</v>
       </c>
@@ -2504,7 +2512,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="68" spans="2:3">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>66</v>
       </c>
@@ -2512,7 +2520,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="69" spans="2:3">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>67</v>
       </c>
@@ -2520,7 +2528,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="70" spans="2:3">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>68</v>
       </c>
@@ -2528,7 +2536,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="71" spans="2:3">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>69</v>
       </c>
@@ -2536,7 +2544,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="72" spans="2:3">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>70</v>
       </c>
@@ -2544,7 +2552,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="73" spans="2:3">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>71</v>
       </c>
@@ -2552,7 +2560,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="74" spans="2:3">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>72</v>
       </c>
@@ -2560,7 +2568,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="75" spans="2:3">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>73</v>
       </c>
@@ -2568,7 +2576,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="76" spans="2:3">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>74</v>
       </c>
@@ -2576,7 +2584,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="77" spans="2:3">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>75</v>
       </c>
@@ -2584,7 +2592,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="78" spans="2:3">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>76</v>
       </c>
@@ -2592,7 +2600,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="79" spans="2:3">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>77</v>
       </c>
@@ -2600,7 +2608,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="80" spans="2:3">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>78</v>
       </c>
@@ -2608,7 +2616,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="81" spans="2:3">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>79</v>
       </c>
@@ -2616,7 +2624,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="82" spans="2:3">
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>80</v>
       </c>
@@ -2624,7 +2632,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="83" spans="2:3">
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>81</v>
       </c>
@@ -2632,7 +2640,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="84" spans="2:3">
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>82</v>
       </c>
@@ -2640,7 +2648,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="85" spans="2:3">
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>83</v>
       </c>
@@ -2648,7 +2656,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="86" spans="2:3">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>84</v>
       </c>
@@ -2656,7 +2664,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="87" spans="2:3">
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>85</v>
       </c>
@@ -2664,7 +2672,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="88" spans="2:3">
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>86</v>
       </c>
@@ -2672,7 +2680,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="89" spans="2:3">
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>87</v>
       </c>
@@ -2680,7 +2688,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="90" spans="2:3">
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>88</v>
       </c>
@@ -2688,7 +2696,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="91" spans="2:3">
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>89</v>
       </c>
@@ -2696,7 +2704,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="92" spans="2:3">
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>90</v>
       </c>
@@ -2704,7 +2712,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="93" spans="2:3">
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>91</v>
       </c>
@@ -2712,7 +2720,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="94" spans="2:3">
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>92</v>
       </c>
@@ -2720,7 +2728,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="95" spans="2:3">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>93</v>
       </c>
@@ -2728,7 +2736,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="96" spans="2:3">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>94</v>
       </c>
@@ -2736,7 +2744,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="97" spans="2:4">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>95</v>
       </c>
@@ -2744,7 +2752,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="98" spans="2:4">
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>96</v>
       </c>
@@ -2752,7 +2760,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="99" spans="2:4">
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>97</v>
       </c>
@@ -2760,7 +2768,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="100" spans="2:4">
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>98</v>
       </c>
@@ -2768,7 +2776,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="101" spans="2:4">
+    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>99</v>
       </c>
@@ -2776,7 +2784,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="102" spans="2:4">
+    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>100</v>
       </c>
@@ -2784,7 +2792,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="103" spans="2:4">
+    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>101</v>
       </c>
@@ -2792,7 +2800,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="104" spans="2:4">
+    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>102</v>
       </c>
@@ -2800,7 +2808,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="105" spans="2:4">
+    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>103</v>
       </c>
@@ -2808,7 +2816,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="106" spans="2:4">
+    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>104</v>
       </c>
@@ -2816,7 +2824,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="107" spans="2:4">
+    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>105</v>
       </c>
@@ -2824,7 +2832,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="108" spans="2:4">
+    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>106</v>
       </c>
@@ -2832,7 +2840,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="109" spans="2:4">
+    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>107</v>
       </c>
@@ -2840,7 +2848,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="110" spans="2:4">
+    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>108</v>
       </c>
@@ -2848,7 +2856,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="111" spans="2:4">
+    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>109</v>
       </c>
@@ -2856,7 +2864,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="112" spans="2:4">
+    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>110</v>
       </c>
@@ -2864,7 +2872,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="113" spans="2:5">
+    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>111</v>
       </c>
@@ -2872,7 +2880,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="114" spans="2:5">
+    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>112</v>
       </c>
@@ -2880,7 +2888,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="115" spans="2:5">
+    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>113</v>
       </c>
@@ -2888,7 +2896,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="116" spans="2:5">
+    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>114</v>
       </c>
@@ -2896,10 +2904,13 @@
         <v>517</v>
       </c>
     </row>
-    <row r="117" spans="2:5">
+    <row r="117" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>115</v>
       </c>
+      <c r="C117" t="s">
+        <v>517</v>
+      </c>
       <c r="D117" t="s">
         <v>527</v>
       </c>
@@ -2907,7 +2918,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="118" spans="2:5">
+    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>116</v>
       </c>
@@ -2915,7 +2926,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="119" spans="2:5">
+    <row r="119" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>117</v>
       </c>
@@ -2923,7 +2934,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="120" spans="2:5">
+    <row r="120" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>118</v>
       </c>
@@ -2931,7 +2942,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="121" spans="2:5">
+    <row r="121" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>119</v>
       </c>
@@ -2939,7 +2950,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="122" spans="2:5">
+    <row r="122" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>120</v>
       </c>
@@ -2947,7 +2958,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="123" spans="2:5">
+    <row r="123" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>121</v>
       </c>
@@ -2955,10 +2966,13 @@
         <v>517</v>
       </c>
     </row>
-    <row r="124" spans="2:5">
+    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>122</v>
       </c>
+      <c r="C124" t="s">
+        <v>517</v>
+      </c>
       <c r="D124" t="s">
         <v>527</v>
       </c>
@@ -2966,7 +2980,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="125" spans="2:5">
+    <row r="125" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>123</v>
       </c>
@@ -2974,7 +2988,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="126" spans="2:5">
+    <row r="126" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>124</v>
       </c>
@@ -2982,7 +2996,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="127" spans="2:5">
+    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>125</v>
       </c>
@@ -2990,7 +3004,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="128" spans="2:5">
+    <row r="128" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>126</v>
       </c>
@@ -2998,7 +3012,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="129" spans="2:3">
+    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>127</v>
       </c>
@@ -3006,7 +3020,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="130" spans="2:3">
+    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>128</v>
       </c>
@@ -3014,7 +3028,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="131" spans="2:3">
+    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>129</v>
       </c>
@@ -3022,7 +3036,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="132" spans="2:3">
+    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>130</v>
       </c>
@@ -3030,7 +3044,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="133" spans="2:3">
+    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
         <v>131</v>
       </c>
@@ -3038,7 +3052,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="134" spans="2:3">
+    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
         <v>132</v>
       </c>
@@ -3046,7 +3060,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="135" spans="2:3">
+    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
         <v>133</v>
       </c>
@@ -3054,7 +3068,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="136" spans="2:3">
+    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
         <v>134</v>
       </c>
@@ -3062,7 +3076,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="137" spans="2:3">
+    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>135</v>
       </c>
@@ -3070,7 +3084,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="138" spans="2:3">
+    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
         <v>136</v>
       </c>
@@ -3078,7 +3092,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="139" spans="2:3">
+    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
         <v>137</v>
       </c>
@@ -3086,7 +3100,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="140" spans="2:3">
+    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
         <v>138</v>
       </c>
@@ -3094,7 +3108,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="141" spans="2:3">
+    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
         <v>139</v>
       </c>
@@ -3102,7 +3116,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="142" spans="2:3">
+    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
         <v>140</v>
       </c>
@@ -3110,7 +3124,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="143" spans="2:3">
+    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
         <v>141</v>
       </c>
@@ -3118,7 +3132,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="144" spans="2:3">
+    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
         <v>142</v>
       </c>
@@ -3126,7 +3140,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="145" spans="2:3">
+    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
         <v>143</v>
       </c>
@@ -3134,7 +3148,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="146" spans="2:3">
+    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
         <v>144</v>
       </c>
@@ -3142,7 +3156,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="147" spans="2:3">
+    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
         <v>145</v>
       </c>
@@ -3150,7 +3164,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="148" spans="2:3">
+    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
         <v>146</v>
       </c>
@@ -3158,7 +3172,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="149" spans="2:3">
+    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
         <v>147</v>
       </c>
@@ -3166,7 +3180,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="150" spans="2:3">
+    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
         <v>148</v>
       </c>
@@ -3174,7 +3188,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="151" spans="2:3">
+    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
         <v>149</v>
       </c>
@@ -3182,7 +3196,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="152" spans="2:3">
+    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
         <v>150</v>
       </c>
@@ -3190,7 +3204,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="153" spans="2:3">
+    <row r="153" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
         <v>151</v>
       </c>
@@ -3198,7 +3212,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="154" spans="2:3">
+    <row r="154" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
         <v>152</v>
       </c>
@@ -3206,7 +3220,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="155" spans="2:3">
+    <row r="155" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
         <v>153</v>
       </c>
@@ -3214,7 +3228,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="156" spans="2:3">
+    <row r="156" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
         <v>154</v>
       </c>
@@ -3222,7 +3236,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="157" spans="2:3">
+    <row r="157" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
         <v>155</v>
       </c>
@@ -3230,7 +3244,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="158" spans="2:3">
+    <row r="158" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
         <v>156</v>
       </c>
@@ -3238,7 +3252,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="159" spans="2:3">
+    <row r="159" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
         <v>157</v>
       </c>
@@ -3246,7 +3260,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="160" spans="2:3">
+    <row r="160" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
         <v>158</v>
       </c>
@@ -3254,7 +3268,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="161" spans="2:5">
+    <row r="161" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
         <v>159</v>
       </c>
@@ -3262,7 +3276,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="162" spans="2:5">
+    <row r="162" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
         <v>160</v>
       </c>
@@ -3270,7 +3284,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="163" spans="2:5">
+    <row r="163" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
         <v>161</v>
       </c>
@@ -3278,7 +3292,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="164" spans="2:5">
+    <row r="164" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
         <v>162</v>
       </c>
@@ -3286,7 +3300,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="165" spans="2:5">
+    <row r="165" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
         <v>163</v>
       </c>
@@ -3294,7 +3308,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="166" spans="2:5">
+    <row r="166" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
         <v>164</v>
       </c>
@@ -3302,10 +3316,13 @@
         <v>517</v>
       </c>
     </row>
-    <row r="167" spans="2:5">
+    <row r="167" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
         <v>165</v>
       </c>
+      <c r="C167" t="s">
+        <v>517</v>
+      </c>
       <c r="D167" t="s">
         <v>529</v>
       </c>
@@ -3313,7 +3330,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="168" spans="2:5">
+    <row r="168" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
         <v>166</v>
       </c>
@@ -3321,7 +3338,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="169" spans="2:5">
+    <row r="169" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
         <v>167</v>
       </c>
@@ -3329,7 +3346,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="170" spans="2:5">
+    <row r="170" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
         <v>168</v>
       </c>
@@ -3337,7 +3354,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="171" spans="2:5">
+    <row r="171" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
         <v>169</v>
       </c>
@@ -3345,7 +3362,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="172" spans="2:5">
+    <row r="172" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
         <v>170</v>
       </c>
@@ -3353,7 +3370,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="173" spans="2:5">
+    <row r="173" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
         <v>171</v>
       </c>
@@ -3361,7 +3378,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="174" spans="2:5">
+    <row r="174" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
         <v>172</v>
       </c>
@@ -3369,7 +3386,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="175" spans="2:5">
+    <row r="175" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
         <v>173</v>
       </c>
@@ -3377,7 +3394,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="176" spans="2:5">
+    <row r="176" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
         <v>174</v>
       </c>
@@ -3385,7 +3402,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="177" spans="2:5">
+    <row r="177" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
         <v>175</v>
       </c>
@@ -3393,7 +3410,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="178" spans="2:5">
+    <row r="178" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
         <v>176</v>
       </c>
@@ -3401,7 +3418,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="179" spans="2:5">
+    <row r="179" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
         <v>177</v>
       </c>
@@ -3409,7 +3426,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="180" spans="2:5">
+    <row r="180" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
         <v>178</v>
       </c>
@@ -3417,7 +3434,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="181" spans="2:5">
+    <row r="181" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
         <v>179</v>
       </c>
@@ -3425,7 +3442,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="182" spans="2:5">
+    <row r="182" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
         <v>180</v>
       </c>
@@ -3433,7 +3450,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="183" spans="2:5">
+    <row r="183" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
         <v>181</v>
       </c>
@@ -3441,7 +3458,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="184" spans="2:5">
+    <row r="184" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
         <v>182</v>
       </c>
@@ -3449,7 +3466,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="185" spans="2:5">
+    <row r="185" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
         <v>183</v>
       </c>
@@ -3457,7 +3474,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="186" spans="2:5">
+    <row r="186" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
         <v>184</v>
       </c>
@@ -3465,7 +3482,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="187" spans="2:5">
+    <row r="187" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
         <v>185</v>
       </c>
@@ -3473,7 +3490,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="188" spans="2:5">
+    <row r="188" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
         <v>186</v>
       </c>
@@ -3481,7 +3498,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="189" spans="2:5">
+    <row r="189" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
         <v>187</v>
       </c>
@@ -3489,7 +3506,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="190" spans="2:5">
+    <row r="190" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
         <v>188</v>
       </c>
@@ -3497,10 +3514,13 @@
         <v>517</v>
       </c>
     </row>
-    <row r="191" spans="2:5">
+    <row r="191" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
         <v>189</v>
       </c>
+      <c r="C191" t="s">
+        <v>517</v>
+      </c>
       <c r="D191" t="s">
         <v>529</v>
       </c>
@@ -3508,7 +3528,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="192" spans="2:5">
+    <row r="192" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
         <v>190</v>
       </c>
@@ -3516,7 +3536,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="193" spans="2:3">
+    <row r="193" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
         <v>191</v>
       </c>
@@ -3524,7 +3544,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="194" spans="2:3">
+    <row r="194" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
         <v>192</v>
       </c>
@@ -3532,7 +3552,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="195" spans="2:3">
+    <row r="195" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
         <v>193</v>
       </c>
@@ -3540,7 +3560,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="196" spans="2:3">
+    <row r="196" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
         <v>194</v>
       </c>
@@ -3548,7 +3568,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="197" spans="2:3">
+    <row r="197" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
         <v>195</v>
       </c>
@@ -3556,7 +3576,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="198" spans="2:3">
+    <row r="198" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
         <v>196</v>
       </c>
@@ -3564,7 +3584,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="199" spans="2:3">
+    <row r="199" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
         <v>197</v>
       </c>
@@ -3572,7 +3592,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="200" spans="2:3">
+    <row r="200" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
         <v>198</v>
       </c>
@@ -3580,7 +3600,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="201" spans="2:3">
+    <row r="201" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
         <v>199</v>
       </c>
@@ -3588,7 +3608,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="202" spans="2:3">
+    <row r="202" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
         <v>200</v>
       </c>
@@ -3596,7 +3616,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="203" spans="2:3">
+    <row r="203" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
         <v>201</v>
       </c>
@@ -3604,7 +3624,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="204" spans="2:3">
+    <row r="204" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B204" t="s">
         <v>202</v>
       </c>
@@ -3612,7 +3632,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="205" spans="2:3">
+    <row r="205" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B205" t="s">
         <v>203</v>
       </c>
@@ -3620,7 +3640,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="206" spans="2:3">
+    <row r="206" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
         <v>204</v>
       </c>
@@ -3628,7 +3648,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="207" spans="2:3">
+    <row r="207" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
         <v>205</v>
       </c>
@@ -3636,7 +3656,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="208" spans="2:3">
+    <row r="208" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
         <v>206</v>
       </c>
@@ -3644,7 +3664,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="209" spans="2:3">
+    <row r="209" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
         <v>207</v>
       </c>
@@ -3652,7 +3672,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="210" spans="2:3">
+    <row r="210" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B210" t="s">
         <v>208</v>
       </c>
@@ -3660,7 +3680,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="211" spans="2:3">
+    <row r="211" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B211" t="s">
         <v>209</v>
       </c>
@@ -3668,7 +3688,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="212" spans="2:3">
+    <row r="212" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
         <v>210</v>
       </c>
@@ -3676,7 +3696,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="213" spans="2:3">
+    <row r="213" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B213" t="s">
         <v>211</v>
       </c>
@@ -3684,7 +3704,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="214" spans="2:3">
+    <row r="214" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B214" t="s">
         <v>212</v>
       </c>
@@ -3692,7 +3712,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="215" spans="2:3">
+    <row r="215" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
         <v>213</v>
       </c>
@@ -3700,7 +3720,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="216" spans="2:3">
+    <row r="216" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
         <v>214</v>
       </c>
@@ -3708,7 +3728,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="217" spans="2:3">
+    <row r="217" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
         <v>215</v>
       </c>
@@ -3716,7 +3736,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="218" spans="2:3">
+    <row r="218" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
         <v>216</v>
       </c>
@@ -3724,7 +3744,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="219" spans="2:3">
+    <row r="219" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B219" t="s">
         <v>217</v>
       </c>
@@ -3732,7 +3752,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="220" spans="2:3">
+    <row r="220" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B220" t="s">
         <v>218</v>
       </c>
@@ -3740,7 +3760,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="221" spans="2:3">
+    <row r="221" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B221" t="s">
         <v>219</v>
       </c>
@@ -3748,7 +3768,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="222" spans="2:3">
+    <row r="222" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
         <v>220</v>
       </c>
@@ -3756,7 +3776,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="223" spans="2:3">
+    <row r="223" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B223" t="s">
         <v>221</v>
       </c>
@@ -3764,7 +3784,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="224" spans="2:3">
+    <row r="224" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B224" t="s">
         <v>222</v>
       </c>
@@ -3772,7 +3792,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="225" spans="2:3">
+    <row r="225" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B225" t="s">
         <v>223</v>
       </c>
@@ -3780,7 +3800,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="226" spans="2:3">
+    <row r="226" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B226" t="s">
         <v>224</v>
       </c>
@@ -3788,7 +3808,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="227" spans="2:3">
+    <row r="227" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B227" t="s">
         <v>225</v>
       </c>
@@ -3796,7 +3816,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="228" spans="2:3">
+    <row r="228" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B228" t="s">
         <v>226</v>
       </c>
@@ -3804,7 +3824,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="229" spans="2:3">
+    <row r="229" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B229" t="s">
         <v>227</v>
       </c>
@@ -3812,7 +3832,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="230" spans="2:3">
+    <row r="230" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B230" t="s">
         <v>228</v>
       </c>
@@ -3820,7 +3840,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="231" spans="2:3">
+    <row r="231" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B231" t="s">
         <v>229</v>
       </c>
@@ -3828,7 +3848,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="232" spans="2:3">
+    <row r="232" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B232" t="s">
         <v>230</v>
       </c>
@@ -3836,7 +3856,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="233" spans="2:3">
+    <row r="233" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B233" t="s">
         <v>231</v>
       </c>
@@ -3844,7 +3864,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="234" spans="2:3">
+    <row r="234" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B234" t="s">
         <v>232</v>
       </c>
@@ -3852,7 +3872,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="235" spans="2:3">
+    <row r="235" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B235" t="s">
         <v>233</v>
       </c>
@@ -3860,7 +3880,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="236" spans="2:3">
+    <row r="236" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B236" t="s">
         <v>234</v>
       </c>
@@ -3868,7 +3888,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="237" spans="2:3">
+    <row r="237" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B237" t="s">
         <v>235</v>
       </c>
@@ -3876,7 +3896,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="238" spans="2:3">
+    <row r="238" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B238" t="s">
         <v>236</v>
       </c>
@@ -3884,7 +3904,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="239" spans="2:3">
+    <row r="239" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B239" t="s">
         <v>237</v>
       </c>
@@ -3892,7 +3912,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="240" spans="2:3">
+    <row r="240" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B240" t="s">
         <v>238</v>
       </c>
@@ -3900,7 +3920,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="241" spans="2:3">
+    <row r="241" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B241" t="s">
         <v>239</v>
       </c>
@@ -3908,7 +3928,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="242" spans="2:3">
+    <row r="242" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B242" t="s">
         <v>240</v>
       </c>
@@ -3916,7 +3936,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="243" spans="2:3">
+    <row r="243" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B243" t="s">
         <v>241</v>
       </c>
@@ -3924,7 +3944,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="244" spans="2:3">
+    <row r="244" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B244" t="s">
         <v>242</v>
       </c>
@@ -3932,7 +3952,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="245" spans="2:3">
+    <row r="245" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B245" t="s">
         <v>243</v>
       </c>
@@ -3940,7 +3960,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="246" spans="2:3">
+    <row r="246" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B246" t="s">
         <v>244</v>
       </c>
@@ -3948,7 +3968,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="247" spans="2:3">
+    <row r="247" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B247" t="s">
         <v>245</v>
       </c>
@@ -3956,7 +3976,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="248" spans="2:3">
+    <row r="248" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B248" t="s">
         <v>246</v>
       </c>
@@ -3964,7 +3984,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="249" spans="2:3">
+    <row r="249" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B249" t="s">
         <v>247</v>
       </c>
@@ -3972,7 +3992,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="250" spans="2:3">
+    <row r="250" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B250" t="s">
         <v>248</v>
       </c>
@@ -3980,7 +4000,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="251" spans="2:3">
+    <row r="251" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B251" t="s">
         <v>249</v>
       </c>
@@ -3988,7 +4008,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="252" spans="2:3">
+    <row r="252" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B252" t="s">
         <v>250</v>
       </c>
@@ -3996,7 +4016,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="253" spans="2:3">
+    <row r="253" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B253" t="s">
         <v>251</v>
       </c>
@@ -4004,7 +4024,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="254" spans="2:3">
+    <row r="254" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B254" t="s">
         <v>252</v>
       </c>
@@ -4012,7 +4032,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="255" spans="2:3">
+    <row r="255" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B255" t="s">
         <v>253</v>
       </c>
@@ -4020,7 +4040,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="256" spans="2:3">
+    <row r="256" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B256" t="s">
         <v>254</v>
       </c>
@@ -4028,7 +4048,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="257" spans="2:3">
+    <row r="257" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B257" t="s">
         <v>255</v>
       </c>
@@ -4036,7 +4056,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="258" spans="2:3">
+    <row r="258" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B258" t="s">
         <v>256</v>
       </c>
@@ -4044,7 +4064,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="259" spans="2:3">
+    <row r="259" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B259" t="s">
         <v>257</v>
       </c>
@@ -4052,7 +4072,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="260" spans="2:3">
+    <row r="260" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B260" t="s">
         <v>258</v>
       </c>
@@ -4060,7 +4080,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="261" spans="2:3">
+    <row r="261" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B261" t="s">
         <v>259</v>
       </c>
@@ -4068,7 +4088,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="262" spans="2:3">
+    <row r="262" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B262" t="s">
         <v>260</v>
       </c>
@@ -4076,7 +4096,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="263" spans="2:3">
+    <row r="263" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B263" t="s">
         <v>261</v>
       </c>
@@ -4084,7 +4104,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="264" spans="2:3">
+    <row r="264" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B264" t="s">
         <v>262</v>
       </c>
@@ -4092,7 +4112,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="265" spans="2:3">
+    <row r="265" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B265" t="s">
         <v>263</v>
       </c>
@@ -4100,7 +4120,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="266" spans="2:3">
+    <row r="266" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B266" t="s">
         <v>264</v>
       </c>
@@ -4108,7 +4128,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="267" spans="2:3">
+    <row r="267" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B267" t="s">
         <v>265</v>
       </c>
@@ -4116,7 +4136,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="268" spans="2:3">
+    <row r="268" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B268" t="s">
         <v>266</v>
       </c>
@@ -4124,7 +4144,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="269" spans="2:3">
+    <row r="269" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B269" t="s">
         <v>267</v>
       </c>
@@ -4132,7 +4152,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="270" spans="2:3">
+    <row r="270" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B270" t="s">
         <v>268</v>
       </c>
@@ -4140,7 +4160,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="271" spans="2:3">
+    <row r="271" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B271" t="s">
         <v>269</v>
       </c>
@@ -4148,7 +4168,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="272" spans="2:3">
+    <row r="272" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B272" t="s">
         <v>270</v>
       </c>
@@ -4156,7 +4176,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="273" spans="2:5">
+    <row r="273" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B273" t="s">
         <v>271</v>
       </c>
@@ -4164,10 +4184,13 @@
         <v>517</v>
       </c>
     </row>
-    <row r="274" spans="2:5">
+    <row r="274" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B274" t="s">
         <v>272</v>
       </c>
+      <c r="C274" t="s">
+        <v>517</v>
+      </c>
       <c r="D274" t="s">
         <v>527</v>
       </c>
@@ -4175,7 +4198,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="275" spans="2:5">
+    <row r="275" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B275" t="s">
         <v>273</v>
       </c>
@@ -4183,7 +4206,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="276" spans="2:5">
+    <row r="276" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B276" t="s">
         <v>274</v>
       </c>
@@ -4191,7 +4214,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="277" spans="2:5">
+    <row r="277" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B277" t="s">
         <v>275</v>
       </c>
@@ -4199,10 +4222,13 @@
         <v>517</v>
       </c>
     </row>
-    <row r="278" spans="2:5">
+    <row r="278" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B278" t="s">
         <v>276</v>
       </c>
+      <c r="C278" t="s">
+        <v>517</v>
+      </c>
       <c r="D278" t="s">
         <v>527</v>
       </c>
@@ -4210,7 +4236,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="279" spans="2:5">
+    <row r="279" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B279" t="s">
         <v>277</v>
       </c>
@@ -4218,7 +4244,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="280" spans="2:5">
+    <row r="280" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B280" t="s">
         <v>278</v>
       </c>
@@ -4226,7 +4252,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="281" spans="2:5">
+    <row r="281" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B281" t="s">
         <v>279</v>
       </c>
@@ -4234,10 +4260,13 @@
         <v>517</v>
       </c>
     </row>
-    <row r="282" spans="2:5">
+    <row r="282" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B282" t="s">
         <v>280</v>
       </c>
+      <c r="C282" t="s">
+        <v>517</v>
+      </c>
       <c r="D282" t="s">
         <v>527</v>
       </c>
@@ -4245,7 +4274,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="283" spans="2:5">
+    <row r="283" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B283" t="s">
         <v>281</v>
       </c>
@@ -4253,7 +4282,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="284" spans="2:5">
+    <row r="284" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B284" t="s">
         <v>282</v>
       </c>
@@ -4261,7 +4290,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="285" spans="2:5">
+    <row r="285" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B285" t="s">
         <v>283</v>
       </c>
@@ -4269,7 +4298,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="286" spans="2:5">
+    <row r="286" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B286" t="s">
         <v>284</v>
       </c>
@@ -4277,7 +4306,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="287" spans="2:5">
+    <row r="287" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B287" t="s">
         <v>285</v>
       </c>
@@ -4285,7 +4314,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="288" spans="2:5">
+    <row r="288" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B288" t="s">
         <v>286</v>
       </c>
@@ -4293,10 +4322,13 @@
         <v>517</v>
       </c>
     </row>
-    <row r="289" spans="2:6">
+    <row r="289" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B289" t="s">
         <v>287</v>
       </c>
+      <c r="C289" t="s">
+        <v>517</v>
+      </c>
       <c r="D289" t="s">
         <v>527</v>
       </c>
@@ -4304,7 +4336,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="290" spans="2:6">
+    <row r="290" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B290" t="s">
         <v>288</v>
       </c>
@@ -4312,7 +4344,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="291" spans="2:6">
+    <row r="291" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B291" t="s">
         <v>289</v>
       </c>
@@ -4320,7 +4352,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="292" spans="2:6">
+    <row r="292" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B292" t="s">
         <v>290</v>
       </c>
@@ -4328,7 +4360,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="293" spans="2:6">
+    <row r="293" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B293" t="s">
         <v>291</v>
       </c>
@@ -4336,7 +4368,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="294" spans="2:6">
+    <row r="294" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B294" t="s">
         <v>292</v>
       </c>
@@ -4344,7 +4376,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="295" spans="2:6">
+    <row r="295" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B295" t="s">
         <v>293</v>
       </c>
@@ -4352,7 +4384,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="296" spans="2:6">
+    <row r="296" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B296" t="s">
         <v>294</v>
       </c>
@@ -4360,7 +4392,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="297" spans="2:6">
+    <row r="297" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B297" t="s">
         <v>295</v>
       </c>
@@ -4368,7 +4400,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="298" spans="2:6">
+    <row r="298" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B298" t="s">
         <v>296</v>
       </c>
@@ -4376,7 +4408,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="299" spans="2:6">
+    <row r="299" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B299" t="s">
         <v>297</v>
       </c>
@@ -4384,10 +4416,13 @@
         <v>517</v>
       </c>
     </row>
-    <row r="300" spans="2:6">
+    <row r="300" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B300" t="s">
         <v>298</v>
       </c>
+      <c r="C300" t="s">
+        <v>517</v>
+      </c>
       <c r="D300" t="s">
         <v>526</v>
       </c>
@@ -4395,10 +4430,13 @@
         <v>536</v>
       </c>
     </row>
-    <row r="301" spans="2:6">
+    <row r="301" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B301" t="s">
         <v>299</v>
       </c>
+      <c r="C301" t="s">
+        <v>517</v>
+      </c>
       <c r="D301" t="s">
         <v>526</v>
       </c>
@@ -4406,7 +4444,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="302" spans="2:6">
+    <row r="302" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B302" t="s">
         <v>300</v>
       </c>
@@ -4414,7 +4452,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="303" spans="2:6">
+    <row r="303" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B303" t="s">
         <v>301</v>
       </c>
@@ -4422,7 +4460,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="304" spans="2:6">
+    <row r="304" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B304" t="s">
         <v>302</v>
       </c>
@@ -4430,7 +4468,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="305" spans="2:3">
+    <row r="305" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B305" t="s">
         <v>0</v>
       </c>
@@ -4438,7 +4476,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="306" spans="2:3">
+    <row r="306" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B306" t="s">
         <v>303</v>
       </c>
@@ -4446,7 +4484,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="307" spans="2:3">
+    <row r="307" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B307" t="s">
         <v>304</v>
       </c>
@@ -4454,7 +4492,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="308" spans="2:3">
+    <row r="308" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B308" t="s">
         <v>305</v>
       </c>
@@ -4462,7 +4500,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="309" spans="2:3">
+    <row r="309" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B309" t="s">
         <v>306</v>
       </c>
@@ -4470,7 +4508,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="310" spans="2:3">
+    <row r="310" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B310" t="s">
         <v>307</v>
       </c>
@@ -4478,7 +4516,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="311" spans="2:3">
+    <row r="311" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B311" t="s">
         <v>308</v>
       </c>
@@ -4486,7 +4524,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="312" spans="2:3">
+    <row r="312" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B312" t="s">
         <v>309</v>
       </c>
@@ -4494,7 +4532,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="313" spans="2:3">
+    <row r="313" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B313" t="s">
         <v>310</v>
       </c>
@@ -4502,7 +4540,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="314" spans="2:3">
+    <row r="314" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B314" t="s">
         <v>311</v>
       </c>
@@ -4510,7 +4548,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="315" spans="2:3">
+    <row r="315" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B315" t="s">
         <v>312</v>
       </c>
@@ -4518,7 +4556,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="316" spans="2:3">
+    <row r="316" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B316" t="s">
         <v>313</v>
       </c>
@@ -4526,7 +4564,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="317" spans="2:3">
+    <row r="317" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B317" t="s">
         <v>314</v>
       </c>
@@ -4534,7 +4572,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="318" spans="2:3">
+    <row r="318" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B318" t="s">
         <v>315</v>
       </c>
@@ -4542,7 +4580,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="319" spans="2:3">
+    <row r="319" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B319" t="s">
         <v>316</v>
       </c>
@@ -4550,7 +4588,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="320" spans="2:3">
+    <row r="320" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B320" t="s">
         <v>317</v>
       </c>
@@ -4558,7 +4596,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="321" spans="2:3">
+    <row r="321" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B321" t="s">
         <v>318</v>
       </c>
@@ -4566,7 +4604,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="322" spans="2:3">
+    <row r="322" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B322" t="s">
         <v>319</v>
       </c>
@@ -4574,7 +4612,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="323" spans="2:3">
+    <row r="323" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B323" t="s">
         <v>320</v>
       </c>
@@ -4582,7 +4620,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="324" spans="2:3">
+    <row r="324" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B324" t="s">
         <v>321</v>
       </c>
@@ -4590,7 +4628,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="325" spans="2:3">
+    <row r="325" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B325" t="s">
         <v>322</v>
       </c>
@@ -4598,7 +4636,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="326" spans="2:3">
+    <row r="326" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B326" t="s">
         <v>323</v>
       </c>
@@ -4606,7 +4644,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="327" spans="2:3">
+    <row r="327" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B327" t="s">
         <v>324</v>
       </c>
@@ -4614,7 +4652,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="328" spans="2:3">
+    <row r="328" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B328" t="s">
         <v>325</v>
       </c>
@@ -4622,7 +4660,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="329" spans="2:3">
+    <row r="329" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B329" t="s">
         <v>326</v>
       </c>
@@ -4630,7 +4668,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="330" spans="2:3">
+    <row r="330" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B330" t="s">
         <v>327</v>
       </c>
@@ -4638,7 +4676,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="331" spans="2:3">
+    <row r="331" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B331" t="s">
         <v>328</v>
       </c>
@@ -4646,7 +4684,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="332" spans="2:3">
+    <row r="332" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B332" t="s">
         <v>329</v>
       </c>
@@ -4654,7 +4692,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="333" spans="2:3">
+    <row r="333" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B333" t="s">
         <v>330</v>
       </c>
@@ -4662,7 +4700,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="334" spans="2:3">
+    <row r="334" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B334" t="s">
         <v>331</v>
       </c>
@@ -4670,7 +4708,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="335" spans="2:3">
+    <row r="335" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B335" t="s">
         <v>332</v>
       </c>
@@ -4678,7 +4716,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="336" spans="2:3">
+    <row r="336" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B336" t="s">
         <v>333</v>
       </c>
@@ -4686,7 +4724,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="337" spans="2:13">
+    <row r="337" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B337" t="s">
         <v>334</v>
       </c>
@@ -4694,7 +4732,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="338" spans="2:13">
+    <row r="338" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B338" t="s">
         <v>335</v>
       </c>
@@ -4702,7 +4740,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="339" spans="2:13">
+    <row r="339" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B339" t="s">
         <v>336</v>
       </c>
@@ -4710,7 +4748,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="340" spans="2:13">
+    <row r="340" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B340" t="s">
         <v>337</v>
       </c>
@@ -4718,7 +4756,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="341" spans="2:13">
+    <row r="341" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B341" t="s">
         <v>338</v>
       </c>
@@ -4726,7 +4764,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="342" spans="2:13">
+    <row r="342" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B342" t="s">
         <v>339</v>
       </c>
@@ -4734,7 +4772,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="343" spans="2:13">
+    <row r="343" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B343" t="s">
         <v>340</v>
       </c>
@@ -4742,7 +4780,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="344" spans="2:13">
+    <row r="344" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B344" t="s">
         <v>341</v>
       </c>
@@ -4750,7 +4788,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="345" spans="2:13">
+    <row r="345" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B345" t="s">
         <v>342</v>
       </c>
@@ -4758,7 +4796,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="346" spans="2:13">
+    <row r="346" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B346" t="s">
         <v>343</v>
       </c>
@@ -4766,10 +4804,13 @@
         <v>517</v>
       </c>
     </row>
-    <row r="347" spans="2:13">
+    <row r="347" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B347" t="s">
         <v>344</v>
       </c>
+      <c r="C347" t="s">
+        <v>517</v>
+      </c>
       <c r="D347" t="s">
         <v>521</v>
       </c>
@@ -4777,7 +4818,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="348" spans="2:13">
+    <row r="348" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B348" t="s">
         <v>345</v>
       </c>
@@ -4785,7 +4826,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="349" spans="2:13">
+    <row r="349" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B349" t="s">
         <v>346</v>
       </c>
@@ -4793,7 +4834,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="350" spans="2:13">
+    <row r="350" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B350" t="s">
         <v>347</v>
       </c>
@@ -4801,7 +4842,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="351" spans="2:13">
+    <row r="351" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B351" t="s">
         <v>348</v>
       </c>
@@ -4809,7 +4850,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="352" spans="2:13">
+    <row r="352" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B352" t="s">
         <v>349</v>
       </c>
@@ -4817,7 +4858,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="353" spans="2:9">
+    <row r="353" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B353" t="s">
         <v>350</v>
       </c>
@@ -4825,7 +4866,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="354" spans="2:9">
+    <row r="354" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B354" t="s">
         <v>351</v>
       </c>
@@ -4833,7 +4874,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="355" spans="2:9">
+    <row r="355" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B355" t="s">
         <v>352</v>
       </c>
@@ -4841,7 +4882,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="356" spans="2:9">
+    <row r="356" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B356" t="s">
         <v>353</v>
       </c>
@@ -4849,7 +4890,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="357" spans="2:9">
+    <row r="357" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B357" t="s">
         <v>354</v>
       </c>
@@ -4857,10 +4898,13 @@
         <v>517</v>
       </c>
     </row>
-    <row r="358" spans="2:9">
+    <row r="358" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B358" t="s">
         <v>355</v>
       </c>
+      <c r="C358" t="s">
+        <v>517</v>
+      </c>
       <c r="D358" t="s">
         <v>525</v>
       </c>
@@ -4868,7 +4912,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="359" spans="2:9">
+    <row r="359" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B359" t="s">
         <v>356</v>
       </c>
@@ -4876,7 +4920,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="360" spans="2:9">
+    <row r="360" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B360" t="s">
         <v>357</v>
       </c>
@@ -4884,7 +4928,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="361" spans="2:9">
+    <row r="361" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B361" t="s">
         <v>358</v>
       </c>
@@ -4892,7 +4936,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="362" spans="2:9">
+    <row r="362" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B362" t="s">
         <v>359</v>
       </c>
@@ -4900,7 +4944,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="363" spans="2:9">
+    <row r="363" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B363" t="s">
         <v>360</v>
       </c>
@@ -4908,7 +4952,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="364" spans="2:9">
+    <row r="364" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B364" t="s">
         <v>361</v>
       </c>
@@ -4916,7 +4960,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="365" spans="2:9">
+    <row r="365" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B365" t="s">
         <v>362</v>
       </c>
@@ -4924,7 +4968,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="366" spans="2:9">
+    <row r="366" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B366" t="s">
         <v>363</v>
       </c>
@@ -4932,7 +4976,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="367" spans="2:9">
+    <row r="367" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B367" t="s">
         <v>364</v>
       </c>
@@ -4940,7 +4984,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="368" spans="2:9">
+    <row r="368" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B368" t="s">
         <v>365</v>
       </c>
@@ -4948,7 +4992,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="369" spans="2:3">
+    <row r="369" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B369" t="s">
         <v>366</v>
       </c>
@@ -4956,7 +5000,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="370" spans="2:3">
+    <row r="370" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B370" t="s">
         <v>367</v>
       </c>
@@ -4964,7 +5008,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="371" spans="2:3">
+    <row r="371" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B371" t="s">
         <v>368</v>
       </c>
@@ -4972,7 +5016,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="372" spans="2:3">
+    <row r="372" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B372" t="s">
         <v>369</v>
       </c>
@@ -4980,7 +5024,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="373" spans="2:3">
+    <row r="373" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B373" t="s">
         <v>370</v>
       </c>
@@ -4988,7 +5032,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="374" spans="2:3">
+    <row r="374" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B374" t="s">
         <v>371</v>
       </c>
@@ -4996,7 +5040,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="375" spans="2:3">
+    <row r="375" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B375" t="s">
         <v>372</v>
       </c>
@@ -5004,7 +5048,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="376" spans="2:3">
+    <row r="376" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B376" t="s">
         <v>373</v>
       </c>
@@ -5012,7 +5056,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="377" spans="2:3">
+    <row r="377" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B377" t="s">
         <v>374</v>
       </c>
@@ -5020,7 +5064,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="378" spans="2:3">
+    <row r="378" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B378" t="s">
         <v>375</v>
       </c>
@@ -5028,7 +5072,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="379" spans="2:3">
+    <row r="379" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B379" t="s">
         <v>376</v>
       </c>
@@ -5036,7 +5080,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="380" spans="2:3">
+    <row r="380" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B380" t="s">
         <v>377</v>
       </c>
@@ -5044,7 +5088,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="381" spans="2:3">
+    <row r="381" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B381" t="s">
         <v>378</v>
       </c>
@@ -5052,7 +5096,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="382" spans="2:3">
+    <row r="382" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B382" t="s">
         <v>379</v>
       </c>
@@ -5060,7 +5104,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="383" spans="2:3">
+    <row r="383" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B383" t="s">
         <v>380</v>
       </c>
@@ -5068,7 +5112,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="384" spans="2:3">
+    <row r="384" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B384" t="s">
         <v>381</v>
       </c>
@@ -5076,7 +5120,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="385" spans="2:3">
+    <row r="385" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B385" t="s">
         <v>382</v>
       </c>
@@ -5084,7 +5128,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="386" spans="2:3">
+    <row r="386" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B386" t="s">
         <v>383</v>
       </c>
@@ -5092,7 +5136,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="387" spans="2:3">
+    <row r="387" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B387" t="s">
         <v>384</v>
       </c>
@@ -5100,7 +5144,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="388" spans="2:3">
+    <row r="388" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B388" t="s">
         <v>385</v>
       </c>
@@ -5108,7 +5152,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="389" spans="2:3">
+    <row r="389" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B389" t="s">
         <v>386</v>
       </c>
@@ -5116,7 +5160,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="390" spans="2:3">
+    <row r="390" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B390" t="s">
         <v>387</v>
       </c>
@@ -5124,7 +5168,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="391" spans="2:3">
+    <row r="391" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B391" t="s">
         <v>388</v>
       </c>
@@ -5132,7 +5176,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="392" spans="2:3">
+    <row r="392" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B392" t="s">
         <v>389</v>
       </c>
@@ -5140,7 +5184,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="393" spans="2:3">
+    <row r="393" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B393" t="s">
         <v>390</v>
       </c>
@@ -5148,7 +5192,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="394" spans="2:3">
+    <row r="394" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B394" t="s">
         <v>391</v>
       </c>
@@ -5156,7 +5200,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="395" spans="2:3">
+    <row r="395" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B395" t="s">
         <v>392</v>
       </c>
@@ -5164,7 +5208,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="396" spans="2:3">
+    <row r="396" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B396" t="s">
         <v>393</v>
       </c>
@@ -5172,7 +5216,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="397" spans="2:3">
+    <row r="397" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B397" t="s">
         <v>394</v>
       </c>
@@ -5180,7 +5224,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="398" spans="2:3">
+    <row r="398" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B398" t="s">
         <v>395</v>
       </c>
@@ -5188,7 +5232,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="399" spans="2:3">
+    <row r="399" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B399" t="s">
         <v>396</v>
       </c>
@@ -5196,7 +5240,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="400" spans="2:3">
+    <row r="400" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B400" t="s">
         <v>397</v>
       </c>
@@ -5204,7 +5248,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="401" spans="2:7">
+    <row r="401" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B401" t="s">
         <v>398</v>
       </c>
@@ -5212,7 +5256,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="402" spans="2:7">
+    <row r="402" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B402" t="s">
         <v>399</v>
       </c>
@@ -5220,7 +5264,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="403" spans="2:7">
+    <row r="403" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B403" t="s">
         <v>400</v>
       </c>
@@ -5228,7 +5272,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="404" spans="2:7">
+    <row r="404" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B404" t="s">
         <v>401</v>
       </c>
@@ -5236,7 +5280,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="405" spans="2:7">
+    <row r="405" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B405" t="s">
         <v>402</v>
       </c>
@@ -5244,7 +5288,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="406" spans="2:7">
+    <row r="406" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B406" t="s">
         <v>403</v>
       </c>
@@ -5252,7 +5296,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="407" spans="2:7">
+    <row r="407" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B407" t="s">
         <v>404</v>
       </c>
@@ -5260,7 +5304,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="408" spans="2:7">
+    <row r="408" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B408" t="s">
         <v>405</v>
       </c>
@@ -5268,7 +5312,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="409" spans="2:7">
+    <row r="409" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B409" t="s">
         <v>406</v>
       </c>
@@ -5276,7 +5320,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="410" spans="2:7">
+    <row r="410" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B410" t="s">
         <v>407</v>
       </c>
@@ -5284,7 +5328,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="411" spans="2:7">
+    <row r="411" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B411" t="s">
         <v>408</v>
       </c>
@@ -5292,7 +5336,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="412" spans="2:7">
+    <row r="412" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B412" t="s">
         <v>409</v>
       </c>
@@ -5300,7 +5344,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="413" spans="2:7">
+    <row r="413" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B413" t="s">
         <v>410</v>
       </c>
@@ -5314,7 +5358,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="414" spans="2:7">
+    <row r="414" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B414" t="s">
         <v>411</v>
       </c>
@@ -5322,7 +5366,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="415" spans="2:7">
+    <row r="415" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B415" t="s">
         <v>412</v>
       </c>
@@ -5330,7 +5374,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="416" spans="2:7">
+    <row r="416" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B416" t="s">
         <v>413</v>
       </c>
@@ -5338,7 +5382,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="417" spans="2:3">
+    <row r="417" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B417" t="s">
         <v>414</v>
       </c>
@@ -5346,7 +5390,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="418" spans="2:3">
+    <row r="418" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B418" t="s">
         <v>415</v>
       </c>
@@ -5354,7 +5398,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="419" spans="2:3">
+    <row r="419" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B419" t="s">
         <v>416</v>
       </c>
@@ -5362,7 +5406,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="420" spans="2:3">
+    <row r="420" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B420" t="s">
         <v>417</v>
       </c>
@@ -5370,7 +5414,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="421" spans="2:3">
+    <row r="421" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B421" t="s">
         <v>418</v>
       </c>
@@ -5378,7 +5422,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="422" spans="2:3">
+    <row r="422" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B422" t="s">
         <v>419</v>
       </c>
@@ -5386,7 +5430,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="423" spans="2:3">
+    <row r="423" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B423" t="s">
         <v>420</v>
       </c>
@@ -5394,7 +5438,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="424" spans="2:3">
+    <row r="424" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B424" t="s">
         <v>421</v>
       </c>
@@ -5402,7 +5446,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="425" spans="2:3">
+    <row r="425" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B425" t="s">
         <v>422</v>
       </c>
@@ -5410,7 +5454,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="426" spans="2:3">
+    <row r="426" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B426" t="s">
         <v>423</v>
       </c>
@@ -5418,7 +5462,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="427" spans="2:3">
+    <row r="427" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B427" t="s">
         <v>424</v>
       </c>
@@ -5426,7 +5470,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="428" spans="2:3">
+    <row r="428" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B428" t="s">
         <v>425</v>
       </c>
@@ -5434,7 +5478,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="429" spans="2:3">
+    <row r="429" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B429" t="s">
         <v>426</v>
       </c>
@@ -5442,7 +5486,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="430" spans="2:3">
+    <row r="430" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B430" t="s">
         <v>427</v>
       </c>
@@ -5450,7 +5494,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="431" spans="2:3">
+    <row r="431" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B431" t="s">
         <v>428</v>
       </c>
@@ -5458,7 +5502,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="432" spans="2:3">
+    <row r="432" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B432" t="s">
         <v>429</v>
       </c>
@@ -5466,7 +5510,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="433" spans="2:3">
+    <row r="433" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B433" t="s">
         <v>430</v>
       </c>
@@ -5474,7 +5518,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="434" spans="2:3">
+    <row r="434" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B434" t="s">
         <v>431</v>
       </c>
@@ -5482,7 +5526,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="435" spans="2:3">
+    <row r="435" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B435" t="s">
         <v>432</v>
       </c>
@@ -5490,7 +5534,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="436" spans="2:3">
+    <row r="436" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B436" t="s">
         <v>433</v>
       </c>
@@ -5498,7 +5542,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="437" spans="2:3">
+    <row r="437" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B437" t="s">
         <v>434</v>
       </c>
@@ -5506,7 +5550,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="438" spans="2:3">
+    <row r="438" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B438" t="s">
         <v>435</v>
       </c>
@@ -5514,7 +5558,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="439" spans="2:3">
+    <row r="439" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B439" t="s">
         <v>436</v>
       </c>
@@ -5522,7 +5566,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="440" spans="2:3">
+    <row r="440" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B440" t="s">
         <v>437</v>
       </c>
@@ -5530,7 +5574,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="441" spans="2:3">
+    <row r="441" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B441" t="s">
         <v>438</v>
       </c>
@@ -5538,7 +5582,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="442" spans="2:3">
+    <row r="442" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B442" t="s">
         <v>439</v>
       </c>
@@ -5546,7 +5590,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="443" spans="2:3">
+    <row r="443" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B443" t="s">
         <v>440</v>
       </c>
@@ -5554,7 +5598,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="444" spans="2:3">
+    <row r="444" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B444" t="s">
         <v>441</v>
       </c>
@@ -5562,7 +5606,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="445" spans="2:3">
+    <row r="445" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B445" t="s">
         <v>442</v>
       </c>
@@ -5570,7 +5614,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="446" spans="2:3">
+    <row r="446" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B446" t="s">
         <v>443</v>
       </c>
@@ -5578,7 +5622,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="447" spans="2:3">
+    <row r="447" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B447" t="s">
         <v>444</v>
       </c>
@@ -5586,7 +5630,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="448" spans="2:3">
+    <row r="448" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B448" t="s">
         <v>445</v>
       </c>
@@ -5594,7 +5638,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="449" spans="2:4">
+    <row r="449" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B449" t="s">
         <v>446</v>
       </c>
@@ -5602,7 +5646,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="450" spans="2:4">
+    <row r="450" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B450" t="s">
         <v>447</v>
       </c>
@@ -5610,7 +5654,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="451" spans="2:4">
+    <row r="451" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B451" t="s">
         <v>448</v>
       </c>
@@ -5618,7 +5662,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="452" spans="2:4">
+    <row r="452" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B452" t="s">
         <v>449</v>
       </c>
@@ -5626,7 +5670,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="453" spans="2:4">
+    <row r="453" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B453" t="s">
         <v>450</v>
       </c>
@@ -5634,7 +5678,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="454" spans="2:4">
+    <row r="454" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B454" t="s">
         <v>451</v>
       </c>
@@ -5642,7 +5686,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="455" spans="2:4">
+    <row r="455" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B455" t="s">
         <v>452</v>
       </c>
@@ -5650,7 +5694,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="456" spans="2:4">
+    <row r="456" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B456" t="s">
         <v>453</v>
       </c>
@@ -5658,7 +5702,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="457" spans="2:4">
+    <row r="457" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B457" t="s">
         <v>454</v>
       </c>
@@ -5666,7 +5710,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="458" spans="2:4">
+    <row r="458" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B458" t="s">
         <v>455</v>
       </c>
@@ -5674,7 +5718,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="459" spans="2:4">
+    <row r="459" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B459" t="s">
         <v>456</v>
       </c>
@@ -5682,7 +5726,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="460" spans="2:4">
+    <row r="460" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B460" t="s">
         <v>457</v>
       </c>
@@ -5690,7 +5734,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="461" spans="2:4">
+    <row r="461" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B461" t="s">
         <v>458</v>
       </c>
@@ -5701,7 +5745,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="462" spans="2:4">
+    <row r="462" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B462" t="s">
         <v>459</v>
       </c>
@@ -5709,7 +5753,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="463" spans="2:4">
+    <row r="463" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B463" t="s">
         <v>460</v>
       </c>
@@ -5717,7 +5761,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="464" spans="2:4">
+    <row r="464" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B464" t="s">
         <v>461</v>
       </c>
@@ -5725,7 +5769,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="465" spans="2:3">
+    <row r="465" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B465" t="s">
         <v>462</v>
       </c>
@@ -5733,7 +5777,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="466" spans="2:3">
+    <row r="466" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B466" t="s">
         <v>463</v>
       </c>
@@ -5741,7 +5785,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="467" spans="2:3">
+    <row r="467" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B467" t="s">
         <v>464</v>
       </c>
@@ -5749,7 +5793,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="468" spans="2:3">
+    <row r="468" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B468" t="s">
         <v>465</v>
       </c>
@@ -5757,7 +5801,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="469" spans="2:3">
+    <row r="469" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B469" t="s">
         <v>466</v>
       </c>
@@ -5765,7 +5809,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="470" spans="2:3">
+    <row r="470" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B470" t="s">
         <v>467</v>
       </c>
@@ -5773,7 +5817,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="471" spans="2:3">
+    <row r="471" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B471" t="s">
         <v>468</v>
       </c>
@@ -5781,7 +5825,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="472" spans="2:3">
+    <row r="472" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B472" t="s">
         <v>469</v>
       </c>
@@ -5789,7 +5833,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="473" spans="2:3">
+    <row r="473" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B473" t="s">
         <v>470</v>
       </c>
@@ -5797,7 +5841,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="474" spans="2:3">
+    <row r="474" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B474" t="s">
         <v>471</v>
       </c>
@@ -5805,7 +5849,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="475" spans="2:3">
+    <row r="475" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B475" t="s">
         <v>472</v>
       </c>
@@ -5813,7 +5857,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="476" spans="2:3">
+    <row r="476" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B476" t="s">
         <v>473</v>
       </c>
@@ -5821,7 +5865,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="477" spans="2:3">
+    <row r="477" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B477" t="s">
         <v>474</v>
       </c>
@@ -5829,7 +5873,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="478" spans="2:3">
+    <row r="478" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B478" t="s">
         <v>475</v>
       </c>
@@ -5837,7 +5881,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="479" spans="2:3">
+    <row r="479" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B479" t="s">
         <v>476</v>
       </c>
@@ -5845,7 +5889,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="480" spans="2:3">
+    <row r="480" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B480" t="s">
         <v>477</v>
       </c>
@@ -5853,7 +5897,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="481" spans="2:3">
+    <row r="481" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B481" t="s">
         <v>478</v>
       </c>
@@ -5861,7 +5905,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="482" spans="2:3">
+    <row r="482" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B482" t="s">
         <v>479</v>
       </c>
@@ -5869,7 +5913,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="483" spans="2:3">
+    <row r="483" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B483" t="s">
         <v>480</v>
       </c>
@@ -5877,7 +5921,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="484" spans="2:3">
+    <row r="484" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B484" t="s">
         <v>481</v>
       </c>
@@ -5885,7 +5929,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="485" spans="2:3">
+    <row r="485" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B485" t="s">
         <v>482</v>
       </c>
@@ -5893,7 +5937,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="486" spans="2:3">
+    <row r="486" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B486" t="s">
         <v>483</v>
       </c>
@@ -5901,7 +5945,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="487" spans="2:3">
+    <row r="487" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B487" t="s">
         <v>484</v>
       </c>
@@ -5909,7 +5953,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="488" spans="2:3">
+    <row r="488" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B488" t="s">
         <v>485</v>
       </c>
@@ -5917,7 +5961,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="489" spans="2:3">
+    <row r="489" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B489" t="s">
         <v>486</v>
       </c>
@@ -5925,7 +5969,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="490" spans="2:3">
+    <row r="490" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B490" t="s">
         <v>487</v>
       </c>
@@ -5933,7 +5977,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="491" spans="2:3">
+    <row r="491" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B491" t="s">
         <v>488</v>
       </c>
@@ -5941,7 +5985,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="492" spans="2:3">
+    <row r="492" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B492" t="s">
         <v>489</v>
       </c>
@@ -5949,7 +5993,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="493" spans="2:3">
+    <row r="493" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B493" t="s">
         <v>490</v>
       </c>
@@ -5957,7 +6001,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="494" spans="2:3">
+    <row r="494" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B494" t="s">
         <v>491</v>
       </c>
@@ -5965,7 +6009,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="495" spans="2:3">
+    <row r="495" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B495" t="s">
         <v>492</v>
       </c>
@@ -5973,7 +6017,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="496" spans="2:3">
+    <row r="496" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B496" t="s">
         <v>493</v>
       </c>
@@ -5981,7 +6025,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="497" spans="2:4">
+    <row r="497" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B497" t="s">
         <v>494</v>
       </c>
@@ -5989,7 +6033,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="498" spans="2:4">
+    <row r="498" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B498" t="s">
         <v>495</v>
       </c>
@@ -5997,7 +6041,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="499" spans="2:4">
+    <row r="499" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B499" t="s">
         <v>496</v>
       </c>
@@ -6005,7 +6049,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="500" spans="2:4">
+    <row r="500" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B500" t="s">
         <v>497</v>
       </c>
@@ -6013,7 +6057,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="501" spans="2:4">
+    <row r="501" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B501" t="s">
         <v>498</v>
       </c>
@@ -6021,7 +6065,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="502" spans="2:4">
+    <row r="502" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B502" t="s">
         <v>499</v>
       </c>
@@ -6029,7 +6073,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="503" spans="2:4">
+    <row r="503" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B503" t="s">
         <v>500</v>
       </c>
@@ -6037,7 +6081,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="504" spans="2:4">
+    <row r="504" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B504" t="s">
         <v>501</v>
       </c>
@@ -6048,7 +6092,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="505" spans="2:4">
+    <row r="505" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B505" t="s">
         <v>502</v>
       </c>
@@ -6056,7 +6100,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="506" spans="2:4">
+    <row r="506" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B506" t="s">
         <v>503</v>
       </c>
@@ -6064,7 +6108,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="507" spans="2:4">
+    <row r="507" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B507" t="s">
         <v>504</v>
       </c>
@@ -6072,7 +6116,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="508" spans="2:4">
+    <row r="508" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B508" t="s">
         <v>505</v>
       </c>
@@ -6080,7 +6124,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="509" spans="2:4">
+    <row r="509" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B509" t="s">
         <v>506</v>
       </c>
@@ -6088,7 +6132,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="510" spans="2:4">
+    <row r="510" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B510" t="s">
         <v>507</v>
       </c>
@@ -6096,7 +6140,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="511" spans="2:4">
+    <row r="511" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B511" t="s">
         <v>508</v>
       </c>
@@ -6104,7 +6148,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="512" spans="2:4">
+    <row r="512" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B512" t="s">
         <v>509</v>
       </c>
@@ -6112,7 +6156,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="513" spans="2:3">
+    <row r="513" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B513" t="s">
         <v>510</v>
       </c>
@@ -6120,7 +6164,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="514" spans="2:3">
+    <row r="514" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B514" t="s">
         <v>511</v>
       </c>
@@ -6128,7 +6172,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="515" spans="2:3">
+    <row r="515" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B515" t="s">
         <v>512</v>
       </c>
@@ -6136,7 +6180,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="516" spans="2:3">
+    <row r="516" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B516" t="s">
         <v>513</v>
       </c>
@@ -6144,7 +6188,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="517" spans="2:3">
+    <row r="517" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B517" t="s">
         <v>514</v>
       </c>
@@ -6152,7 +6196,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="518" spans="2:3">
+    <row r="518" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B518" t="s">
         <v>515</v>
       </c>

</xml_diff>

<commit_message>
id anchoring orgName partial
</commit_message>
<xml_diff>
--- a/Kate.CheckList.MT.xlsx
+++ b/Kate.CheckList.MT.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="593">
   <si>
     <t>MpÃ©pe (1)</t>
   </si>
@@ -1586,39 +1586,12 @@
     <t>y1</t>
   </si>
   <si>
-    <t>liv_000099_0004 is Robert the</t>
-  </si>
-  <si>
-    <t>corrected</t>
-  </si>
-  <si>
-    <t>KS has marked this person as at 0572. Check with JL whether Mr Wilkes is the same copy editor as Wilkes.</t>
-  </si>
-  <si>
-    <t>One of two names of a company</t>
-  </si>
-  <si>
     <t>y (I think)</t>
   </si>
   <si>
-    <t>marked as above, query check</t>
-  </si>
-  <si>
-    <t>query check, spelling in glossary is Mwata Yamvo</t>
-  </si>
-  <si>
-    <t>Query check</t>
-  </si>
-  <si>
-    <t>Query</t>
-  </si>
-  <si>
     <t>ND</t>
   </si>
   <si>
-    <t>query</t>
-  </si>
-  <si>
     <t>add id for Sekote</t>
   </si>
   <si>
@@ -1650,13 +1623,196 @@
   </si>
   <si>
     <t>Use Id for Mwant Yav</t>
+  </si>
+  <si>
+    <t>orgName</t>
+  </si>
+  <si>
+    <t>aboriginal (2)</t>
+  </si>
+  <si>
+    <t>Admiralty (8)</t>
+  </si>
+  <si>
+    <t>Algerine Arabs (1)</t>
+  </si>
+  <si>
+    <t>AnnatolansAnatolians (1)</t>
+  </si>
+  <si>
+    <t>Baptist (1)</t>
+  </si>
+  <si>
+    <t>British and Portuguese mixed commission at Cape town (1)</t>
+  </si>
+  <si>
+    <t>British Museum (1)</t>
+  </si>
+  <si>
+    <t>Cape Observatory (1)</t>
+  </si>
+  <si>
+    <t>Chartist (1)</t>
+  </si>
+  <si>
+    <t>church missionaryChurch Missionary (1)</t>
+  </si>
+  <si>
+    <t>Circassians (1)</t>
+  </si>
+  <si>
+    <t>Coldstreams (1)</t>
+  </si>
+  <si>
+    <t>Covenanters (1)</t>
+  </si>
+  <si>
+    <t>Dutch Reformed (2)</t>
+  </si>
+  <si>
+    <t>Empacasseiros (1)</t>
+  </si>
+  <si>
+    <t>Enniskillens (1)</t>
+  </si>
+  <si>
+    <t>Episcopalian (1)</t>
+  </si>
+  <si>
+    <t>Faculty of Physicians and Surgeons (1)</t>
+  </si>
+  <si>
+    <t>German legion (1)</t>
+  </si>
+  <si>
+    <t>Government House Cape town (1)</t>
+  </si>
+  <si>
+    <t>Griqua (5)</t>
+  </si>
+  <si>
+    <t>Hottentots (14)</t>
+  </si>
+  <si>
+    <t>IndependantIndependent (1)</t>
+  </si>
+  <si>
+    <t>Jesuit (1)</t>
+  </si>
+  <si>
+    <t>Knights of Malta (1)</t>
+  </si>
+  <si>
+    <t>light cavalry (1)</t>
+  </si>
+  <si>
+    <t>Locrians (1)</t>
+  </si>
+  <si>
+    <t>London Missionary Society (3)</t>
+  </si>
+  <si>
+    <t>Lords of the islesIsles (1)</t>
+  </si>
+  <si>
+    <t>Madras army (1)</t>
+  </si>
+  <si>
+    <t>Mansion House of London (1)</t>
+  </si>
+  <si>
+    <t>Mantatees (1)</t>
+  </si>
+  <si>
+    <t>Mechanics InstituteMechanics' Institute (1)</t>
+  </si>
+  <si>
+    <t>Monteith &amp; Co. (1)</t>
+  </si>
+  <si>
+    <t>Mopato (5)</t>
+  </si>
+  <si>
+    <t>Moravians (1)</t>
+  </si>
+  <si>
+    <t>Niger Expedition (1)</t>
+  </si>
+  <si>
+    <t>peace society (1)</t>
+  </si>
+  <si>
+    <t>Presbyterian (1)</t>
+  </si>
+  <si>
+    <t>Quakers (1)</t>
+  </si>
+  <si>
+    <t>resurrectionist (1)</t>
+  </si>
+  <si>
+    <t>Rhenish (1)</t>
+  </si>
+  <si>
+    <t>Royal Geographical society (1)</t>
+  </si>
+  <si>
+    <t>South Sea Islanders (1)</t>
+  </si>
+  <si>
+    <t>St Mary's Woolnoth (1)</t>
+  </si>
+  <si>
+    <t>Thames Steamer (1)</t>
+  </si>
+  <si>
+    <t>Thracians (1)</t>
+  </si>
+  <si>
+    <t>Troughton and Sims (1)</t>
+  </si>
+  <si>
+    <t>United Presbyterian church (1)</t>
+  </si>
+  <si>
+    <t>University of Coimbra (1)</t>
+  </si>
+  <si>
+    <t>Wesleyans (1)</t>
+  </si>
+  <si>
+    <t>Westminster (1)</t>
+  </si>
+  <si>
+    <t>Zambesians (1)</t>
+  </si>
+  <si>
+    <t>Makalaka (19)</t>
+  </si>
+  <si>
+    <t>persName</t>
+  </si>
+  <si>
+    <t>African Portuguese (1) and Native Portuguese (6)</t>
+  </si>
+  <si>
+    <t>Ambacistas (3) actual (4) corrected &lt;tribe&gt; error</t>
+  </si>
+  <si>
+    <t>Boers (75) Dutch African (1) and Boerish (1)</t>
+  </si>
+  <si>
+    <t>Bushmen (43) and variants</t>
+  </si>
+  <si>
+    <t>Caffre (26) and variants</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1664,16 +1820,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1681,12 +1864,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1967,263 +2193,419 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M518"/>
+  <dimension ref="B1:M518"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40.5703125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="8" t="s">
+        <v>587</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="E2" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="E3" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="9" t="s">
+        <v>588</v>
+      </c>
+      <c r="E4" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="E5" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="3" t="s">
+        <v>589</v>
+      </c>
+      <c r="E6" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="E7" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="E8" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="10" t="s">
+        <v>590</v>
+      </c>
+      <c r="E9" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="E10" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="E11" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="10" t="s">
+        <v>591</v>
+      </c>
+      <c r="E12" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="10" t="s">
+        <v>592</v>
+      </c>
+      <c r="E13" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>12</v>
       </c>
       <c r="C14" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="E14" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>13</v>
       </c>
       <c r="C15" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="E15" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>14</v>
       </c>
       <c r="C16" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="E16" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>15</v>
       </c>
       <c r="C17" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="E17" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>16</v>
       </c>
       <c r="C18" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="E18" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>17</v>
       </c>
       <c r="C19" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="E19" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>18</v>
       </c>
       <c r="C20" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>19</v>
       </c>
       <c r="C21" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="2" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>20</v>
       </c>
       <c r="C22" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="5" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>21</v>
       </c>
       <c r="C23" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="2" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>22</v>
       </c>
       <c r="C24" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="4" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>23</v>
       </c>
       <c r="C25" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="2" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>24</v>
       </c>
       <c r="C26" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="2" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>25</v>
       </c>
       <c r="C27" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="4" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>26</v>
       </c>
       <c r="C28" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="2" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>27</v>
       </c>
       <c r="C29" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="4" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>28</v>
       </c>
       <c r="C30" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="4" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>29</v>
       </c>
       <c r="C31" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="2" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>30</v>
       </c>
       <c r="C32" t="s">
         <v>517</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
@@ -2233,8 +2615,8 @@
       <c r="C33" t="s">
         <v>518</v>
       </c>
-      <c r="D33" t="s">
-        <v>519</v>
+      <c r="D33" s="3" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
@@ -2244,6 +2626,9 @@
       <c r="C34" t="s">
         <v>517</v>
       </c>
+      <c r="D34" s="2" t="s">
+        <v>559</v>
+      </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
@@ -2252,6 +2637,9 @@
       <c r="C35" t="s">
         <v>517</v>
       </c>
+      <c r="D35" s="2" t="s">
+        <v>560</v>
+      </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
@@ -2260,6 +2648,9 @@
       <c r="C36" t="s">
         <v>517</v>
       </c>
+      <c r="D36" s="3" t="s">
+        <v>561</v>
+      </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
@@ -2268,6 +2659,9 @@
       <c r="C37" t="s">
         <v>517</v>
       </c>
+      <c r="D37" s="2" t="s">
+        <v>562</v>
+      </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
@@ -2276,6 +2670,9 @@
       <c r="C38" t="s">
         <v>517</v>
       </c>
+      <c r="D38" s="2" t="s">
+        <v>563</v>
+      </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
@@ -2284,6 +2681,9 @@
       <c r="C39" t="s">
         <v>517</v>
       </c>
+      <c r="D39" s="2" t="s">
+        <v>564</v>
+      </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
@@ -2292,6 +2692,9 @@
       <c r="C40" t="s">
         <v>517</v>
       </c>
+      <c r="D40" s="2" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
@@ -2300,6 +2703,9 @@
       <c r="C41" t="s">
         <v>517</v>
       </c>
+      <c r="D41" s="2" t="s">
+        <v>566</v>
+      </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
@@ -2308,6 +2714,9 @@
       <c r="C42" t="s">
         <v>517</v>
       </c>
+      <c r="D42" s="2" t="s">
+        <v>567</v>
+      </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
@@ -2316,6 +2725,9 @@
       <c r="C43" t="s">
         <v>517</v>
       </c>
+      <c r="D43" s="4" t="s">
+        <v>568</v>
+      </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
@@ -2324,6 +2736,9 @@
       <c r="C44" t="s">
         <v>517</v>
       </c>
+      <c r="D44" s="3" t="s">
+        <v>569</v>
+      </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
@@ -2332,6 +2747,9 @@
       <c r="C45" t="s">
         <v>517</v>
       </c>
+      <c r="D45" s="3" t="s">
+        <v>570</v>
+      </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
@@ -2340,6 +2758,9 @@
       <c r="C46" t="s">
         <v>517</v>
       </c>
+      <c r="D46" s="4" t="s">
+        <v>571</v>
+      </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
@@ -2348,6 +2769,9 @@
       <c r="C47" t="s">
         <v>517</v>
       </c>
+      <c r="D47" s="2" t="s">
+        <v>572</v>
+      </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
@@ -2356,6 +2780,9 @@
       <c r="C48" t="s">
         <v>517</v>
       </c>
+      <c r="D48" s="3" t="s">
+        <v>573</v>
+      </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
@@ -2364,6 +2791,9 @@
       <c r="C49" t="s">
         <v>517</v>
       </c>
+      <c r="D49" s="4" t="s">
+        <v>574</v>
+      </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
@@ -2372,6 +2802,9 @@
       <c r="C50" t="s">
         <v>517</v>
       </c>
+      <c r="D50" s="2" t="s">
+        <v>575</v>
+      </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
@@ -2380,6 +2813,9 @@
       <c r="C51" t="s">
         <v>517</v>
       </c>
+      <c r="D51" s="2" t="s">
+        <v>576</v>
+      </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
@@ -2388,6 +2824,9 @@
       <c r="C52" t="s">
         <v>517</v>
       </c>
+      <c r="D52" s="2" t="s">
+        <v>577</v>
+      </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
@@ -2396,6 +2835,9 @@
       <c r="C53" t="s">
         <v>517</v>
       </c>
+      <c r="D53" s="2" t="s">
+        <v>578</v>
+      </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
@@ -2404,6 +2846,9 @@
       <c r="C54" t="s">
         <v>517</v>
       </c>
+      <c r="D54" s="3" t="s">
+        <v>579</v>
+      </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
@@ -2412,6 +2857,9 @@
       <c r="C55" t="s">
         <v>517</v>
       </c>
+      <c r="D55" s="2" t="s">
+        <v>580</v>
+      </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
@@ -2420,6 +2868,9 @@
       <c r="C56" t="s">
         <v>517</v>
       </c>
+      <c r="D56" s="4" t="s">
+        <v>581</v>
+      </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
@@ -2428,6 +2879,9 @@
       <c r="C57" t="s">
         <v>517</v>
       </c>
+      <c r="D57" s="3" t="s">
+        <v>582</v>
+      </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
@@ -2436,6 +2890,9 @@
       <c r="C58" t="s">
         <v>517</v>
       </c>
+      <c r="D58" s="2" t="s">
+        <v>583</v>
+      </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
@@ -2444,6 +2901,9 @@
       <c r="C59" t="s">
         <v>517</v>
       </c>
+      <c r="D59" s="4" t="s">
+        <v>584</v>
+      </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
@@ -2452,6 +2912,9 @@
       <c r="C60" t="s">
         <v>517</v>
       </c>
+      <c r="D60" s="4" t="s">
+        <v>585</v>
+      </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
@@ -2468,9 +2931,6 @@
       <c r="C62" t="s">
         <v>517</v>
       </c>
-      <c r="D62" t="s">
-        <v>520</v>
-      </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
@@ -2487,6 +2947,9 @@
       <c r="C64" t="s">
         <v>517</v>
       </c>
+      <c r="D64" s="7" t="s">
+        <v>586</v>
+      </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
@@ -2744,7 +3207,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>95</v>
       </c>
@@ -2752,7 +3215,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>96</v>
       </c>
@@ -2760,7 +3223,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>97</v>
       </c>
@@ -2768,7 +3231,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>98</v>
       </c>
@@ -2776,15 +3239,12 @@
         <v>517</v>
       </c>
     </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>99</v>
       </c>
-      <c r="D101" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>100</v>
       </c>
@@ -2792,7 +3252,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>101</v>
       </c>
@@ -2800,7 +3260,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>102</v>
       </c>
@@ -2808,7 +3268,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>103</v>
       </c>
@@ -2816,7 +3276,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>104</v>
       </c>
@@ -2824,7 +3284,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>105</v>
       </c>
@@ -2832,7 +3292,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>106</v>
       </c>
@@ -2840,7 +3300,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>107</v>
       </c>
@@ -2848,7 +3308,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>108</v>
       </c>
@@ -2856,7 +3316,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>109</v>
       </c>
@@ -2864,7 +3324,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>110</v>
       </c>
@@ -2911,11 +3371,8 @@
       <c r="C117" t="s">
         <v>517</v>
       </c>
-      <c r="D117" t="s">
-        <v>527</v>
-      </c>
       <c r="E117" t="s">
-        <v>530</v>
+        <v>521</v>
       </c>
     </row>
     <row r="118" spans="2:5" x14ac:dyDescent="0.25">
@@ -2973,11 +3430,8 @@
       <c r="C124" t="s">
         <v>517</v>
       </c>
-      <c r="D124" t="s">
-        <v>527</v>
-      </c>
       <c r="E124" t="s">
-        <v>531</v>
+        <v>522</v>
       </c>
     </row>
     <row r="125" spans="2:5" x14ac:dyDescent="0.25">
@@ -3073,7 +3527,7 @@
         <v>134</v>
       </c>
       <c r="C136" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
@@ -3081,7 +3535,7 @@
         <v>135</v>
       </c>
       <c r="C137" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
@@ -3097,7 +3551,7 @@
         <v>137</v>
       </c>
       <c r="C139" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.25">
@@ -3323,11 +3777,8 @@
       <c r="C167" t="s">
         <v>517</v>
       </c>
-      <c r="D167" t="s">
-        <v>529</v>
-      </c>
       <c r="E167" t="s">
-        <v>532</v>
+        <v>523</v>
       </c>
     </row>
     <row r="168" spans="2:5" x14ac:dyDescent="0.25">
@@ -3463,7 +3914,7 @@
         <v>182</v>
       </c>
       <c r="C184" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
     </row>
     <row r="185" spans="2:5" x14ac:dyDescent="0.25">
@@ -3471,7 +3922,7 @@
         <v>183</v>
       </c>
       <c r="C185" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
     </row>
     <row r="186" spans="2:5" x14ac:dyDescent="0.25">
@@ -3521,11 +3972,8 @@
       <c r="C191" t="s">
         <v>517</v>
       </c>
-      <c r="D191" t="s">
-        <v>529</v>
-      </c>
       <c r="E191" t="s">
-        <v>532</v>
+        <v>523</v>
       </c>
     </row>
     <row r="192" spans="2:5" x14ac:dyDescent="0.25">
@@ -3685,7 +4133,7 @@
         <v>209</v>
       </c>
       <c r="C211" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
     </row>
     <row r="212" spans="2:3" x14ac:dyDescent="0.25">
@@ -3965,7 +4413,7 @@
         <v>244</v>
       </c>
       <c r="C246" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
     </row>
     <row r="247" spans="2:3" x14ac:dyDescent="0.25">
@@ -4191,11 +4639,8 @@
       <c r="C274" t="s">
         <v>517</v>
       </c>
-      <c r="D274" t="s">
-        <v>527</v>
-      </c>
       <c r="E274" t="s">
-        <v>533</v>
+        <v>524</v>
       </c>
     </row>
     <row r="275" spans="2:5" x14ac:dyDescent="0.25">
@@ -4229,11 +4674,8 @@
       <c r="C278" t="s">
         <v>517</v>
       </c>
-      <c r="D278" t="s">
-        <v>527</v>
-      </c>
       <c r="E278" t="s">
-        <v>533</v>
+        <v>524</v>
       </c>
     </row>
     <row r="279" spans="2:5" x14ac:dyDescent="0.25">
@@ -4267,11 +4709,8 @@
       <c r="C282" t="s">
         <v>517</v>
       </c>
-      <c r="D282" t="s">
-        <v>527</v>
-      </c>
       <c r="E282" t="s">
-        <v>534</v>
+        <v>525</v>
       </c>
     </row>
     <row r="283" spans="2:5" x14ac:dyDescent="0.25">
@@ -4329,11 +4768,8 @@
       <c r="C289" t="s">
         <v>517</v>
       </c>
-      <c r="D289" t="s">
-        <v>527</v>
-      </c>
       <c r="E289" t="s">
-        <v>535</v>
+        <v>526</v>
       </c>
     </row>
     <row r="290" spans="2:6" x14ac:dyDescent="0.25">
@@ -4423,11 +4859,8 @@
       <c r="C300" t="s">
         <v>517</v>
       </c>
-      <c r="D300" t="s">
-        <v>526</v>
-      </c>
       <c r="F300" t="s">
-        <v>536</v>
+        <v>527</v>
       </c>
     </row>
     <row r="301" spans="2:6" x14ac:dyDescent="0.25">
@@ -4437,11 +4870,8 @@
       <c r="C301" t="s">
         <v>517</v>
       </c>
-      <c r="D301" t="s">
-        <v>526</v>
-      </c>
       <c r="F301" t="s">
-        <v>537</v>
+        <v>528</v>
       </c>
     </row>
     <row r="302" spans="2:6" x14ac:dyDescent="0.25">
@@ -4811,11 +5241,8 @@
       <c r="C347" t="s">
         <v>517</v>
       </c>
-      <c r="D347" t="s">
-        <v>521</v>
-      </c>
       <c r="M347" t="s">
-        <v>538</v>
+        <v>529</v>
       </c>
     </row>
     <row r="348" spans="2:13" x14ac:dyDescent="0.25">
@@ -4905,11 +5332,8 @@
       <c r="C358" t="s">
         <v>517</v>
       </c>
-      <c r="D358" t="s">
-        <v>525</v>
-      </c>
       <c r="I358" t="s">
-        <v>540</v>
+        <v>531</v>
       </c>
     </row>
     <row r="359" spans="2:9" x14ac:dyDescent="0.25">
@@ -5197,7 +5621,7 @@
         <v>391</v>
       </c>
       <c r="C394" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
     </row>
     <row r="395" spans="2:3" x14ac:dyDescent="0.25">
@@ -5351,11 +5775,8 @@
       <c r="C413" t="s">
         <v>517</v>
       </c>
-      <c r="D413" t="s">
-        <v>524</v>
-      </c>
       <c r="G413" t="s">
-        <v>539</v>
+        <v>530</v>
       </c>
     </row>
     <row r="414" spans="2:7" x14ac:dyDescent="0.25">
@@ -5638,7 +6059,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="449" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="449" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B449" t="s">
         <v>446</v>
       </c>
@@ -5646,7 +6067,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="450" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="450" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B450" t="s">
         <v>447</v>
       </c>
@@ -5654,7 +6075,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="451" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="451" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B451" t="s">
         <v>448</v>
       </c>
@@ -5662,7 +6083,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="452" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="452" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B452" t="s">
         <v>449</v>
       </c>
@@ -5670,7 +6091,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="453" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="453" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B453" t="s">
         <v>450</v>
       </c>
@@ -5678,7 +6099,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="454" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="454" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B454" t="s">
         <v>451</v>
       </c>
@@ -5686,7 +6107,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="455" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="455" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B455" t="s">
         <v>452</v>
       </c>
@@ -5694,7 +6115,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="456" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="456" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B456" t="s">
         <v>453</v>
       </c>
@@ -5702,7 +6123,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="457" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="457" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B457" t="s">
         <v>454</v>
       </c>
@@ -5710,7 +6131,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="458" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="458" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B458" t="s">
         <v>455</v>
       </c>
@@ -5718,7 +6139,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="459" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="459" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B459" t="s">
         <v>456</v>
       </c>
@@ -5726,7 +6147,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="460" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="460" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B460" t="s">
         <v>457</v>
       </c>
@@ -5734,18 +6155,15 @@
         <v>517</v>
       </c>
     </row>
-    <row r="461" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="461" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B461" t="s">
         <v>458</v>
       </c>
       <c r="C461" t="s">
-        <v>528</v>
-      </c>
-      <c r="D461" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="462" spans="2:4" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="462" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B462" t="s">
         <v>459</v>
       </c>
@@ -5753,7 +6171,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="463" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="463" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B463" t="s">
         <v>460</v>
       </c>
@@ -5761,7 +6179,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="464" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="464" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B464" t="s">
         <v>461</v>
       </c>
@@ -6025,7 +6443,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="497" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="497" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B497" t="s">
         <v>494</v>
       </c>
@@ -6033,7 +6451,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="498" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="498" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B498" t="s">
         <v>495</v>
       </c>
@@ -6041,7 +6459,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="499" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="499" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B499" t="s">
         <v>496</v>
       </c>
@@ -6049,7 +6467,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="500" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="500" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B500" t="s">
         <v>497</v>
       </c>
@@ -6057,7 +6475,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="501" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="501" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B501" t="s">
         <v>498</v>
       </c>
@@ -6065,7 +6483,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="502" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="502" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B502" t="s">
         <v>499</v>
       </c>
@@ -6073,7 +6491,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="503" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="503" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B503" t="s">
         <v>500</v>
       </c>
@@ -6081,18 +6499,15 @@
         <v>517</v>
       </c>
     </row>
-    <row r="504" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="504" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B504" t="s">
         <v>501</v>
       </c>
       <c r="C504" t="s">
-        <v>528</v>
-      </c>
-      <c r="D504" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="505" spans="2:4" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="505" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B505" t="s">
         <v>502</v>
       </c>
@@ -6100,7 +6515,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="506" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="506" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B506" t="s">
         <v>503</v>
       </c>
@@ -6108,7 +6523,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="507" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="507" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B507" t="s">
         <v>504</v>
       </c>
@@ -6116,7 +6531,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="508" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="508" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B508" t="s">
         <v>505</v>
       </c>
@@ -6124,7 +6539,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="509" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="509" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B509" t="s">
         <v>506</v>
       </c>
@@ -6132,7 +6547,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="510" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="510" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B510" t="s">
         <v>507</v>
       </c>
@@ -6140,7 +6555,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="511" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="511" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B511" t="s">
         <v>508</v>
       </c>
@@ -6148,7 +6563,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="512" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="512" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B512" t="s">
         <v>509</v>
       </c>
@@ -6206,6 +6621,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
orgName ID list complete
</commit_message>
<xml_diff>
--- a/Kate.CheckList.MT.xlsx
+++ b/Kate.CheckList.MT.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="594">
   <si>
     <t>MpÃ©pe (1)</t>
   </si>
@@ -1688,9 +1688,6 @@
     <t>Government House Cape town (1)</t>
   </si>
   <si>
-    <t>Griqua (5)</t>
-  </si>
-  <si>
     <t>Hottentots (14)</t>
   </si>
   <si>
@@ -1806,6 +1803,12 @@
   </si>
   <si>
     <t>Caffre (26) and variants</t>
+  </si>
+  <si>
+    <t>Griqua (5) and variants</t>
+  </si>
+  <si>
+    <t>checked</t>
   </si>
 </sst>
 </file>
@@ -2195,8 +2198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M518"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="C56" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2207,7 +2210,7 @@
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>532</v>
@@ -2249,7 +2252,7 @@
         <v>517</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="E4" t="s">
         <v>517</v>
@@ -2277,7 +2280,7 @@
         <v>517</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E6" t="s">
         <v>517</v>
@@ -2319,7 +2322,7 @@
         <v>517</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="E9" t="s">
         <v>517</v>
@@ -2361,7 +2364,7 @@
         <v>517</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E12" t="s">
         <v>517</v>
@@ -2375,7 +2378,7 @@
         <v>517</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E13" t="s">
         <v>517</v>
@@ -2475,6 +2478,9 @@
       <c r="D20" s="2" t="s">
         <v>99</v>
       </c>
+      <c r="E20" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
@@ -2486,6 +2492,9 @@
       <c r="D21" s="2" t="s">
         <v>546</v>
       </c>
+      <c r="E21" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
@@ -2497,6 +2506,9 @@
       <c r="D22" s="5" t="s">
         <v>547</v>
       </c>
+      <c r="E22" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
@@ -2508,6 +2520,9 @@
       <c r="D23" s="2" t="s">
         <v>548</v>
       </c>
+      <c r="E23" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
@@ -2519,6 +2534,9 @@
       <c r="D24" s="4" t="s">
         <v>549</v>
       </c>
+      <c r="E24" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
@@ -2530,6 +2548,9 @@
       <c r="D25" s="2" t="s">
         <v>550</v>
       </c>
+      <c r="E25" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
@@ -2541,6 +2562,9 @@
       <c r="D26" s="2" t="s">
         <v>551</v>
       </c>
+      <c r="E26" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
@@ -2552,6 +2576,9 @@
       <c r="D27" s="4" t="s">
         <v>552</v>
       </c>
+      <c r="E27" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
@@ -2560,8 +2587,11 @@
       <c r="C28" t="s">
         <v>517</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>553</v>
+      <c r="D28" s="10" t="s">
+        <v>592</v>
+      </c>
+      <c r="E28" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
@@ -2572,7 +2602,10 @@
         <v>517</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>554</v>
+        <v>553</v>
+      </c>
+      <c r="E29" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
@@ -2583,7 +2616,10 @@
         <v>517</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>555</v>
+        <v>554</v>
+      </c>
+      <c r="E30" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
@@ -2594,7 +2630,10 @@
         <v>517</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
+      </c>
+      <c r="E31" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
@@ -2605,10 +2644,13 @@
         <v>517</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+        <v>556</v>
+      </c>
+      <c r="E32" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>31</v>
       </c>
@@ -2616,10 +2658,13 @@
         <v>518</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+        <v>557</v>
+      </c>
+      <c r="E33" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>32</v>
       </c>
@@ -2627,10 +2672,13 @@
         <v>517</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+        <v>558</v>
+      </c>
+      <c r="E34" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>33</v>
       </c>
@@ -2638,10 +2686,13 @@
         <v>517</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+      <c r="E35" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>34</v>
       </c>
@@ -2649,10 +2700,13 @@
         <v>517</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+        <v>560</v>
+      </c>
+      <c r="E36" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>35</v>
       </c>
@@ -2660,10 +2714,13 @@
         <v>517</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="E37" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>36</v>
       </c>
@@ -2671,10 +2728,13 @@
         <v>517</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+        <v>562</v>
+      </c>
+      <c r="E38" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>37</v>
       </c>
@@ -2682,10 +2742,13 @@
         <v>517</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+        <v>563</v>
+      </c>
+      <c r="E39" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>38</v>
       </c>
@@ -2693,10 +2756,13 @@
         <v>517</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+        <v>564</v>
+      </c>
+      <c r="E40" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>39</v>
       </c>
@@ -2704,10 +2770,13 @@
         <v>517</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+        <v>565</v>
+      </c>
+      <c r="E41" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>40</v>
       </c>
@@ -2715,10 +2784,13 @@
         <v>517</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+        <v>566</v>
+      </c>
+      <c r="E42" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>41</v>
       </c>
@@ -2726,10 +2798,13 @@
         <v>517</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+        <v>567</v>
+      </c>
+      <c r="E43" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>42</v>
       </c>
@@ -2737,10 +2812,13 @@
         <v>517</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+        <v>568</v>
+      </c>
+      <c r="E44" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>43</v>
       </c>
@@ -2748,10 +2826,13 @@
         <v>517</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+        <v>569</v>
+      </c>
+      <c r="E45" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>44</v>
       </c>
@@ -2759,10 +2840,13 @@
         <v>517</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+        <v>570</v>
+      </c>
+      <c r="E46" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>45</v>
       </c>
@@ -2770,10 +2854,13 @@
         <v>517</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+        <v>571</v>
+      </c>
+      <c r="E47" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>46</v>
       </c>
@@ -2781,10 +2868,13 @@
         <v>517</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+        <v>572</v>
+      </c>
+      <c r="E48" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>47</v>
       </c>
@@ -2792,10 +2882,13 @@
         <v>517</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+        <v>573</v>
+      </c>
+      <c r="E49" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>48</v>
       </c>
@@ -2803,10 +2896,13 @@
         <v>517</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+        <v>574</v>
+      </c>
+      <c r="E50" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>49</v>
       </c>
@@ -2814,10 +2910,13 @@
         <v>517</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+        <v>575</v>
+      </c>
+      <c r="E51" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>50</v>
       </c>
@@ -2825,10 +2924,13 @@
         <v>517</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+        <v>576</v>
+      </c>
+      <c r="E52" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>51</v>
       </c>
@@ -2836,10 +2938,13 @@
         <v>517</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+        <v>577</v>
+      </c>
+      <c r="E53" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>52</v>
       </c>
@@ -2847,10 +2952,13 @@
         <v>517</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+        <v>578</v>
+      </c>
+      <c r="E54" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>53</v>
       </c>
@@ -2858,10 +2966,13 @@
         <v>517</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+        <v>579</v>
+      </c>
+      <c r="E55" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>54</v>
       </c>
@@ -2869,10 +2980,13 @@
         <v>517</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+        <v>580</v>
+      </c>
+      <c r="E56" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>55</v>
       </c>
@@ -2880,10 +2994,13 @@
         <v>517</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+        <v>581</v>
+      </c>
+      <c r="E57" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>56</v>
       </c>
@@ -2891,10 +3008,13 @@
         <v>517</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+        <v>582</v>
+      </c>
+      <c r="E58" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>57</v>
       </c>
@@ -2902,10 +3022,13 @@
         <v>517</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+        <v>583</v>
+      </c>
+      <c r="E59" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>58</v>
       </c>
@@ -2913,10 +3036,13 @@
         <v>517</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+        <v>584</v>
+      </c>
+      <c r="E60" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>59</v>
       </c>
@@ -2924,7 +3050,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>60</v>
       </c>
@@ -2932,7 +3058,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>61</v>
       </c>
@@ -2940,7 +3066,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>62</v>
       </c>
@@ -2948,7 +3074,10 @@
         <v>517</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>586</v>
+        <v>585</v>
+      </c>
+      <c r="E64" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>